<commit_message>
Update lại Tasksheet.xlsx và Use case/Basic Use Case Diagram - Use Case.png #LongDB
</commit_message>
<xml_diff>
--- a/wiki/report/Tasksheet.xlsx
+++ b/wiki/report/Tasksheet.xlsx
@@ -124,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="126">
   <si>
     <t>No.</t>
   </si>
@@ -725,7 +725,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -852,6 +852,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="9"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1155,11 +1158,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L115"/>
+  <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="12" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A102" sqref="A102:A107"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="12" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F51" sqref="F45:F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1815,14 +1818,14 @@
       <c r="A34" s="42"/>
       <c r="B34" s="46"/>
       <c r="C34" s="30" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="D34" s="32"/>
-      <c r="E34" s="37" t="s">
-        <v>8</v>
-      </c>
+      <c r="E34" s="37"/>
       <c r="F34" s="32"/>
-      <c r="G34" s="32"/>
+      <c r="G34" s="32" t="s">
+        <v>8</v>
+      </c>
       <c r="H34" s="40"/>
       <c r="I34" s="14"/>
       <c r="J34" s="14"/>
@@ -1835,7 +1838,7 @@
       <c r="A35" s="42"/>
       <c r="B35" s="46"/>
       <c r="C35" s="30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D35" s="32"/>
       <c r="E35" s="32" t="s">
@@ -1854,10 +1857,13 @@
     <row r="36" spans="1:12" ht="15.75">
       <c r="A36" s="42"/>
       <c r="B36" s="46"/>
-      <c r="C36" s="31" t="s">
-        <v>96</v>
+      <c r="C36" s="30" t="s">
+        <v>95</v>
       </c>
       <c r="D36" s="32"/>
+      <c r="E36" s="32" t="s">
+        <v>8</v>
+      </c>
       <c r="F36" s="32"/>
       <c r="G36" s="32"/>
       <c r="H36" s="40">
@@ -1871,13 +1877,11 @@
     <row r="37" spans="1:12" ht="15.75">
       <c r="A37" s="42"/>
       <c r="B37" s="46"/>
-      <c r="C37" s="30" t="s">
-        <v>97</v>
+      <c r="C37" s="31" t="s">
+        <v>96</v>
       </c>
       <c r="D37" s="32"/>
-      <c r="E37" s="37" t="s">
-        <v>8</v>
-      </c>
+      <c r="E37" s="37"/>
       <c r="F37" s="32"/>
       <c r="G37" s="32"/>
       <c r="H37" s="40"/>
@@ -1892,7 +1896,7 @@
       <c r="A38" s="42"/>
       <c r="B38" s="46"/>
       <c r="C38" s="30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D38" s="32"/>
       <c r="E38" s="32" t="s">
@@ -1912,7 +1916,7 @@
       <c r="A39" s="42"/>
       <c r="B39" s="46"/>
       <c r="C39" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D39" s="32"/>
       <c r="E39" s="32" t="s">
@@ -1932,7 +1936,7 @@
       <c r="A40" s="42"/>
       <c r="B40" s="46"/>
       <c r="C40" s="30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D40" s="32"/>
       <c r="E40" s="32" t="s">
@@ -1952,7 +1956,7 @@
       <c r="A41" s="42"/>
       <c r="B41" s="46"/>
       <c r="C41" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D41" s="32"/>
       <c r="E41" s="32" t="s">
@@ -1971,11 +1975,13 @@
     <row r="42" spans="1:12" ht="15.75">
       <c r="A42" s="42"/>
       <c r="B42" s="46"/>
-      <c r="C42" s="31" t="s">
-        <v>102</v>
+      <c r="C42" s="30" t="s">
+        <v>101</v>
       </c>
       <c r="D42" s="32"/>
-      <c r="E42" s="32"/>
+      <c r="E42" s="32" t="s">
+        <v>8</v>
+      </c>
       <c r="G42" s="32"/>
       <c r="H42" s="40">
         <v>21</v>
@@ -1988,14 +1994,14 @@
     <row r="43" spans="1:12" ht="15.75">
       <c r="A43" s="42"/>
       <c r="B43" s="46"/>
-      <c r="C43" s="30" t="s">
-        <v>103</v>
+      <c r="C43" s="51" t="s">
+        <v>109</v>
       </c>
       <c r="D43" s="32"/>
-      <c r="E43" s="32"/>
-      <c r="F43" s="37" t="s">
-        <v>8</v>
-      </c>
+      <c r="E43" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="F43" s="37"/>
       <c r="G43" s="32"/>
       <c r="H43" s="40"/>
       <c r="I43" s="14"/>
@@ -2008,14 +2014,12 @@
     <row r="44" spans="1:12" ht="15.75">
       <c r="A44" s="42"/>
       <c r="B44" s="46"/>
-      <c r="C44" s="30" t="s">
-        <v>104</v>
+      <c r="C44" s="31" t="s">
+        <v>102</v>
       </c>
       <c r="D44" s="32"/>
       <c r="E44" s="32"/>
-      <c r="F44" s="32" t="s">
-        <v>8</v>
-      </c>
+      <c r="F44" s="32"/>
       <c r="G44" s="32"/>
       <c r="H44" s="40"/>
       <c r="I44" s="14"/>
@@ -2029,7 +2033,7 @@
       <c r="A45" s="42"/>
       <c r="B45" s="46"/>
       <c r="C45" s="30" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D45" s="32"/>
       <c r="E45" s="32"/>
@@ -2049,7 +2053,7 @@
       <c r="A46" s="42"/>
       <c r="B46" s="46"/>
       <c r="C46" s="30" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D46" s="32"/>
       <c r="E46" s="32"/>
@@ -2069,7 +2073,7 @@
       <c r="A47" s="42"/>
       <c r="B47" s="46"/>
       <c r="C47" s="30" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D47" s="32"/>
       <c r="E47" s="32"/>
@@ -2089,7 +2093,7 @@
       <c r="A48" s="42"/>
       <c r="B48" s="46"/>
       <c r="C48" s="30" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D48" s="32"/>
       <c r="E48" s="32"/>
@@ -2109,7 +2113,7 @@
       <c r="A49" s="42"/>
       <c r="B49" s="46"/>
       <c r="C49" s="30" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D49" s="32"/>
       <c r="E49" s="32"/>
@@ -2129,7 +2133,7 @@
       <c r="A50" s="42"/>
       <c r="B50" s="46"/>
       <c r="C50" s="30" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D50" s="32"/>
       <c r="E50" s="32"/>
@@ -2149,7 +2153,7 @@
       <c r="A51" s="42"/>
       <c r="B51" s="46"/>
       <c r="C51" s="30" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D51" s="32"/>
       <c r="E51" s="32"/>
@@ -2169,13 +2173,13 @@
       <c r="A52" s="42"/>
       <c r="B52" s="46"/>
       <c r="C52" s="30" t="s">
-        <v>112</v>
-      </c>
-      <c r="D52" s="32"/>
+        <v>110</v>
+      </c>
+      <c r="D52" s="32" t="s">
+        <v>8</v>
+      </c>
       <c r="E52" s="32"/>
-      <c r="F52" s="32" t="s">
-        <v>8</v>
-      </c>
+      <c r="F52" s="32"/>
       <c r="G52" s="32"/>
       <c r="H52" s="40"/>
       <c r="I52" s="14"/>
@@ -2189,7 +2193,7 @@
       <c r="A53" s="42"/>
       <c r="B53" s="46"/>
       <c r="C53" s="30" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D53" s="32" t="s">
         <v>8</v>
@@ -2209,7 +2213,7 @@
       <c r="A54" s="42"/>
       <c r="B54" s="46"/>
       <c r="C54" s="30" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D54" s="32" t="s">
         <v>8</v>
@@ -2229,7 +2233,7 @@
       <c r="A55" s="42"/>
       <c r="B55" s="46"/>
       <c r="C55" s="30" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D55" s="32" t="s">
         <v>8</v>
@@ -2249,7 +2253,7 @@
       <c r="A56" s="42"/>
       <c r="B56" s="46"/>
       <c r="C56" s="30" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D56" s="32" t="s">
         <v>8</v>
@@ -2269,7 +2273,7 @@
       <c r="A57" s="42"/>
       <c r="B57" s="46"/>
       <c r="C57" s="30" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D57" s="32" t="s">
         <v>8</v>
@@ -2289,7 +2293,7 @@
       <c r="A58" s="42"/>
       <c r="B58" s="46"/>
       <c r="C58" s="30" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D58" s="32" t="s">
         <v>8</v>
@@ -2309,7 +2313,7 @@
       <c r="A59" s="42"/>
       <c r="B59" s="46"/>
       <c r="C59" s="30" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D59" s="32" t="s">
         <v>8</v>
@@ -2329,7 +2333,7 @@
       <c r="A60" s="42"/>
       <c r="B60" s="46"/>
       <c r="C60" s="30" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D60" s="32" t="s">
         <v>8</v>
@@ -2349,7 +2353,7 @@
       <c r="A61" s="42"/>
       <c r="B61" s="46"/>
       <c r="C61" s="30" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D61" s="32" t="s">
         <v>8</v>
@@ -2369,12 +2373,12 @@
       <c r="A62" s="42"/>
       <c r="B62" s="46"/>
       <c r="C62" s="30" t="s">
-        <v>122</v>
-      </c>
-      <c r="D62" s="32"/>
-      <c r="E62" s="32" t="s">
-        <v>8</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="D62" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62" s="32"/>
       <c r="F62" s="32"/>
       <c r="G62" s="32"/>
       <c r="H62" s="40"/>
@@ -2389,12 +2393,12 @@
       <c r="A63" s="42"/>
       <c r="B63" s="46"/>
       <c r="C63" s="30" t="s">
-        <v>123</v>
-      </c>
-      <c r="D63" s="2"/>
-      <c r="E63" s="2" t="s">
-        <v>8</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E63" s="2"/>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
       <c r="H63" s="40"/>
@@ -2408,11 +2412,13 @@
     <row r="64" spans="1:12" ht="15.75">
       <c r="A64" s="42"/>
       <c r="B64" s="46"/>
-      <c r="C64" s="7" t="s">
-        <v>21</v>
+      <c r="C64" s="30" t="s">
+        <v>122</v>
       </c>
       <c r="D64" s="2"/>
-      <c r="E64" s="2"/>
+      <c r="E64" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
       <c r="H64" s="40"/>
@@ -2426,11 +2432,13 @@
     <row r="65" spans="1:12" ht="15.75">
       <c r="A65" s="42"/>
       <c r="B65" s="46"/>
-      <c r="C65" s="8" t="s">
-        <v>22</v>
+      <c r="C65" s="30" t="s">
+        <v>123</v>
       </c>
       <c r="D65" s="2"/>
-      <c r="E65" s="2"/>
+      <c r="E65" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
       <c r="H65" s="40"/>
@@ -2442,8 +2450,8 @@
     <row r="66" spans="1:12" ht="15.75">
       <c r="A66" s="42"/>
       <c r="B66" s="46"/>
-      <c r="C66" s="8" t="s">
-        <v>23</v>
+      <c r="C66" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
@@ -2459,7 +2467,7 @@
       <c r="A67" s="42"/>
       <c r="B67" s="46"/>
       <c r="C67" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
@@ -2474,8 +2482,8 @@
     <row r="68" spans="1:12" ht="15.75">
       <c r="A68" s="43"/>
       <c r="B68" s="47"/>
-      <c r="C68" s="9" t="s">
-        <v>25</v>
+      <c r="C68" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
@@ -2494,8 +2502,8 @@
       <c r="B69" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="C69" s="4" t="s">
-        <v>26</v>
+      <c r="C69" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
@@ -2510,8 +2518,8 @@
     <row r="70" spans="1:12" ht="15.75">
       <c r="A70" s="42"/>
       <c r="B70" s="42"/>
-      <c r="C70" s="4" t="s">
-        <v>53</v>
+      <c r="C70" s="9" t="s">
+        <v>25</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
@@ -2526,8 +2534,8 @@
     <row r="71" spans="1:12" ht="15.75">
       <c r="A71" s="42"/>
       <c r="B71" s="42"/>
-      <c r="C71" s="10" t="s">
-        <v>54</v>
+      <c r="C71" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
@@ -2542,8 +2550,8 @@
     <row r="72" spans="1:12" ht="15.75">
       <c r="A72" s="42"/>
       <c r="B72" s="42"/>
-      <c r="C72" s="11" t="s">
-        <v>55</v>
+      <c r="C72" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
@@ -2558,8 +2566,8 @@
     <row r="73" spans="1:12" ht="15.75">
       <c r="A73" s="42"/>
       <c r="B73" s="42"/>
-      <c r="C73" s="11" t="s">
-        <v>56</v>
+      <c r="C73" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
@@ -2574,8 +2582,8 @@
     <row r="74" spans="1:12" ht="15.75">
       <c r="A74" s="42"/>
       <c r="B74" s="42"/>
-      <c r="C74" s="12" t="s">
-        <v>27</v>
+      <c r="C74" s="11" t="s">
+        <v>55</v>
       </c>
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
@@ -2590,8 +2598,8 @@
     <row r="75" spans="1:12" ht="15.75">
       <c r="A75" s="42"/>
       <c r="B75" s="42"/>
-      <c r="C75" s="10" t="s">
-        <v>28</v>
+      <c r="C75" s="11" t="s">
+        <v>56</v>
       </c>
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
@@ -2606,8 +2614,8 @@
     <row r="76" spans="1:12" ht="15.75">
       <c r="A76" s="42"/>
       <c r="B76" s="42"/>
-      <c r="C76" s="11" t="s">
-        <v>29</v>
+      <c r="C76" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
@@ -2622,8 +2630,8 @@
     <row r="77" spans="1:12" ht="15.75">
       <c r="A77" s="42"/>
       <c r="B77" s="42"/>
-      <c r="C77" s="11" t="s">
-        <v>30</v>
+      <c r="C77" s="10" t="s">
+        <v>28</v>
       </c>
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
@@ -2638,8 +2646,8 @@
     <row r="78" spans="1:12" ht="15.75">
       <c r="A78" s="42"/>
       <c r="B78" s="42"/>
-      <c r="C78" s="13" t="s">
-        <v>31</v>
+      <c r="C78" s="11" t="s">
+        <v>29</v>
       </c>
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
@@ -2654,8 +2662,8 @@
     <row r="79" spans="1:12" ht="15.75" customHeight="1">
       <c r="A79" s="42"/>
       <c r="B79" s="42"/>
-      <c r="C79" s="8" t="s">
-        <v>50</v>
+      <c r="C79" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
@@ -2670,8 +2678,8 @@
     <row r="80" spans="1:12" ht="15.75">
       <c r="A80" s="42"/>
       <c r="B80" s="42"/>
-      <c r="C80" s="8" t="s">
-        <v>51</v>
+      <c r="C80" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="D80" s="2"/>
       <c r="E80" s="2"/>
@@ -2687,7 +2695,7 @@
       <c r="A81" s="42"/>
       <c r="B81" s="42"/>
       <c r="C81" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
@@ -2702,8 +2710,8 @@
     <row r="82" spans="1:12" ht="15.75">
       <c r="A82" s="42"/>
       <c r="B82" s="42"/>
-      <c r="C82" s="13" t="s">
-        <v>48</v>
+      <c r="C82" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
@@ -2718,8 +2726,8 @@
     <row r="83" spans="1:12" ht="15.75">
       <c r="A83" s="43"/>
       <c r="B83" s="43"/>
-      <c r="C83" s="13" t="s">
-        <v>49</v>
+      <c r="C83" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
@@ -2738,8 +2746,8 @@
       <c r="B84" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="C84" s="5" t="s">
-        <v>40</v>
+      <c r="C84" s="13" t="s">
+        <v>48</v>
       </c>
       <c r="D84" s="2"/>
       <c r="E84" s="2"/>
@@ -2754,8 +2762,8 @@
     <row r="85" spans="1:12" ht="15.75">
       <c r="A85" s="49"/>
       <c r="B85" s="42"/>
-      <c r="C85" s="5" t="s">
-        <v>32</v>
+      <c r="C85" s="13" t="s">
+        <v>49</v>
       </c>
       <c r="D85" s="2"/>
       <c r="E85" s="2"/>
@@ -2770,8 +2778,8 @@
     <row r="86" spans="1:12" ht="15.75">
       <c r="A86" s="49"/>
       <c r="B86" s="42"/>
-      <c r="C86" s="11" t="s">
-        <v>34</v>
+      <c r="C86" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="D86" s="2"/>
       <c r="E86" s="2"/>
@@ -2786,8 +2794,8 @@
     <row r="87" spans="1:12" ht="15.75">
       <c r="A87" s="49"/>
       <c r="B87" s="42"/>
-      <c r="C87" s="11" t="s">
-        <v>35</v>
+      <c r="C87" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="D87" s="2"/>
       <c r="E87" s="2"/>
@@ -2802,8 +2810,8 @@
     <row r="88" spans="1:12" ht="15.75">
       <c r="A88" s="49"/>
       <c r="B88" s="42"/>
-      <c r="C88" s="5" t="s">
-        <v>33</v>
+      <c r="C88" s="11" t="s">
+        <v>34</v>
       </c>
       <c r="D88" s="2"/>
       <c r="E88" s="2"/>
@@ -2819,7 +2827,7 @@
       <c r="A89" s="49"/>
       <c r="B89" s="42"/>
       <c r="C89" s="11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D89" s="2"/>
       <c r="E89" s="2"/>
@@ -2834,8 +2842,8 @@
     <row r="90" spans="1:12" ht="15.75">
       <c r="A90" s="49"/>
       <c r="B90" s="42"/>
-      <c r="C90" s="11" t="s">
-        <v>35</v>
+      <c r="C90" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="D90" s="2"/>
       <c r="E90" s="2"/>
@@ -2850,8 +2858,8 @@
     <row r="91" spans="1:12" ht="15.75">
       <c r="A91" s="49"/>
       <c r="B91" s="42"/>
-      <c r="C91" s="4" t="s">
-        <v>59</v>
+      <c r="C91" s="11" t="s">
+        <v>34</v>
       </c>
       <c r="D91" s="2"/>
       <c r="E91" s="2"/>
@@ -2866,8 +2874,8 @@
     <row r="92" spans="1:12" ht="15.75">
       <c r="A92" s="49"/>
       <c r="B92" s="42"/>
-      <c r="C92" s="13" t="s">
-        <v>36</v>
+      <c r="C92" s="11" t="s">
+        <v>35</v>
       </c>
       <c r="D92" s="2"/>
       <c r="E92" s="2"/>
@@ -2882,8 +2890,8 @@
     <row r="93" spans="1:12" ht="15.75">
       <c r="A93" s="49"/>
       <c r="B93" s="42"/>
-      <c r="C93" s="11" t="s">
-        <v>20</v>
+      <c r="C93" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="D93" s="2"/>
       <c r="E93" s="2"/>
@@ -2898,8 +2906,8 @@
     <row r="94" spans="1:12" ht="15.75" customHeight="1">
       <c r="A94" s="49"/>
       <c r="B94" s="42"/>
-      <c r="C94" s="11" t="s">
-        <v>38</v>
+      <c r="C94" s="13" t="s">
+        <v>36</v>
       </c>
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
@@ -2915,7 +2923,7 @@
       <c r="A95" s="49"/>
       <c r="B95" s="42"/>
       <c r="C95" s="11" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="D95" s="2"/>
       <c r="E95" s="2"/>
@@ -2930,8 +2938,8 @@
     <row r="96" spans="1:12" ht="15.75">
       <c r="A96" s="49"/>
       <c r="B96" s="42"/>
-      <c r="C96" s="13" t="s">
-        <v>37</v>
+      <c r="C96" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="D96" s="2"/>
       <c r="E96" s="2"/>
@@ -2947,7 +2955,7 @@
       <c r="A97" s="49"/>
       <c r="B97" s="42"/>
       <c r="C97" s="11" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="D97" s="2"/>
       <c r="E97" s="2"/>
@@ -2962,8 +2970,8 @@
     <row r="98" spans="1:12" ht="15.75">
       <c r="A98" s="49"/>
       <c r="B98" s="42"/>
-      <c r="C98" s="11" t="s">
-        <v>38</v>
+      <c r="C98" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="D98" s="2"/>
       <c r="E98" s="2"/>
@@ -2978,8 +2986,8 @@
     <row r="99" spans="1:12" ht="15.75">
       <c r="A99" s="49"/>
       <c r="B99" s="42"/>
-      <c r="C99" s="13" t="s">
-        <v>57</v>
+      <c r="C99" s="11" t="s">
+        <v>20</v>
       </c>
       <c r="D99" s="2"/>
       <c r="E99" s="2"/>
@@ -2995,7 +3003,7 @@
       <c r="A100" s="49"/>
       <c r="B100" s="42"/>
       <c r="C100" s="11" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D100" s="2"/>
       <c r="E100" s="2"/>
@@ -3010,8 +3018,8 @@
     <row r="101" spans="1:12" ht="15.75">
       <c r="A101" s="50"/>
       <c r="B101" s="43"/>
-      <c r="C101" s="11" t="s">
-        <v>38</v>
+      <c r="C101" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
@@ -3030,8 +3038,8 @@
       <c r="B102" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="C102" s="13" t="s">
-        <v>41</v>
+      <c r="C102" s="11" t="s">
+        <v>20</v>
       </c>
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
@@ -3046,8 +3054,8 @@
     <row r="103" spans="1:12" ht="15.75">
       <c r="A103" s="49"/>
       <c r="B103" s="42"/>
-      <c r="C103" s="13" t="s">
-        <v>42</v>
+      <c r="C103" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
@@ -3062,8 +3070,8 @@
     <row r="104" spans="1:12" ht="15.75">
       <c r="A104" s="49"/>
       <c r="B104" s="42"/>
-      <c r="C104" s="11" t="s">
-        <v>20</v>
+      <c r="C104" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="D104" s="2"/>
       <c r="E104" s="2"/>
@@ -3078,8 +3086,8 @@
     <row r="105" spans="1:12" ht="15.75">
       <c r="A105" s="49"/>
       <c r="B105" s="42"/>
-      <c r="C105" s="11" t="s">
-        <v>38</v>
+      <c r="C105" s="13" t="s">
+        <v>42</v>
       </c>
       <c r="D105" s="2"/>
       <c r="E105" s="2"/>
@@ -3095,7 +3103,7 @@
       <c r="A106" s="49"/>
       <c r="B106" s="42"/>
       <c r="C106" s="11" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="D106" s="2"/>
       <c r="E106" s="2"/>
@@ -3110,8 +3118,8 @@
     <row r="107" spans="1:12" ht="15.75">
       <c r="A107" s="50"/>
       <c r="B107" s="43"/>
-      <c r="C107" s="13" t="s">
-        <v>43</v>
+      <c r="C107" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="D107" s="2"/>
       <c r="E107" s="2"/>
@@ -3126,7 +3134,9 @@
     <row r="108" spans="1:12">
       <c r="A108" s="3"/>
       <c r="B108" s="3"/>
-      <c r="C108" s="1"/>
+      <c r="C108" s="11" t="s">
+        <v>39</v>
+      </c>
       <c r="D108" s="3"/>
       <c r="E108" s="3"/>
       <c r="F108" s="3"/>
@@ -3141,7 +3151,9 @@
         <v>62</v>
       </c>
       <c r="B109" s="3"/>
-      <c r="C109" s="1"/>
+      <c r="C109" s="13" t="s">
+        <v>43</v>
+      </c>
       <c r="D109" s="3"/>
       <c r="E109" s="3"/>
       <c r="F109" s="3"/>
@@ -3158,9 +3170,7 @@
       <c r="B110" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="C110" s="4" t="s">
-        <v>64</v>
-      </c>
+      <c r="C110" s="1"/>
       <c r="D110" s="3"/>
       <c r="E110" s="3"/>
       <c r="F110" s="3"/>
@@ -3177,9 +3187,7 @@
       <c r="B111" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C111" s="4">
-        <v>1</v>
-      </c>
+      <c r="C111" s="1"/>
       <c r="D111" s="3"/>
       <c r="E111" s="3"/>
       <c r="F111" s="3"/>
@@ -3196,8 +3204,8 @@
       <c r="B112" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="C112" s="21">
-        <v>2</v>
+      <c r="C112" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="D112" s="3"/>
       <c r="E112" s="3"/>
@@ -3215,8 +3223,8 @@
       <c r="B113" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C113" s="21">
-        <v>3</v>
+      <c r="C113" s="4">
+        <v>1</v>
       </c>
       <c r="D113" s="3"/>
       <c r="E113" s="3"/>
@@ -3235,7 +3243,7 @@
         <v>69</v>
       </c>
       <c r="C114" s="21">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D114" s="3"/>
       <c r="E114" s="3"/>
@@ -3254,7 +3262,7 @@
         <v>68</v>
       </c>
       <c r="C115" s="21">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D115" s="3"/>
       <c r="E115" s="3"/>
@@ -3264,6 +3272,16 @@
       <c r="J115" s="3"/>
       <c r="K115" s="3"/>
       <c r="L115" s="36"/>
+    </row>
+    <row r="116" spans="1:12">
+      <c r="C116" s="21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12">
+      <c r="C117" s="21">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -3281,7 +3299,7 @@
     <mergeCell ref="A102:A107"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L30 G42 E37:E115 F43:G115 D2:D115 F2:G41 E2:E32 E34:E35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L30 G42 F43:G115 D2:D115 F2:G41 E2:E32 E34:E115">
       <formula1>"O, "</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update lại Report 3 - Software Requirement Specification.docx và Tasksheet.xlsx #LongDB
</commit_message>
<xml_diff>
--- a/wiki/report/Tasksheet.xlsx
+++ b/wiki/report/Tasksheet.xlsx
@@ -124,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="127">
   <si>
     <t>No.</t>
   </si>
@@ -502,6 +502,9 @@
   </si>
   <si>
     <t>Use-case specification</t>
+  </si>
+  <si>
+    <t>Search information</t>
   </si>
 </sst>
 </file>
@@ -731,7 +734,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -826,36 +829,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="9"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="7"/>
@@ -871,6 +844,47 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="9"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1173,11 +1187,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L117"/>
+  <dimension ref="A1:L118"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="12" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C45" sqref="C45:C65"/>
+      <pane ySplit="12" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1195,7 +1209,7 @@
     <col min="12" max="12" width="7.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="28.5">
+    <row r="1" spans="1:12" ht="18.75">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -1234,10 +1248,10 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75" hidden="1">
-      <c r="A2" s="42">
+      <c r="A2" s="49">
         <v>1</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="49" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -1256,8 +1270,8 @@
       <c r="L2" s="30"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" hidden="1">
-      <c r="A3" s="43"/>
-      <c r="B3" s="43"/>
+      <c r="A3" s="50"/>
+      <c r="B3" s="50"/>
       <c r="C3" s="4" t="s">
         <v>45</v>
       </c>
@@ -1274,8 +1288,8 @@
       <c r="L3" s="30"/>
     </row>
     <row r="4" spans="1:12" ht="15.75" hidden="1">
-      <c r="A4" s="43"/>
-      <c r="B4" s="43"/>
+      <c r="A4" s="50"/>
+      <c r="B4" s="50"/>
       <c r="C4" s="4" t="s">
         <v>46</v>
       </c>
@@ -1292,8 +1306,8 @@
       <c r="L4" s="30"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" hidden="1">
-      <c r="A5" s="43"/>
-      <c r="B5" s="43"/>
+      <c r="A5" s="50"/>
+      <c r="B5" s="50"/>
       <c r="C5" s="4" t="s">
         <v>47</v>
       </c>
@@ -1312,8 +1326,8 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" hidden="1">
-      <c r="A6" s="43"/>
-      <c r="B6" s="43"/>
+      <c r="A6" s="50"/>
+      <c r="B6" s="50"/>
       <c r="C6" s="4" t="s">
         <v>12</v>
       </c>
@@ -1328,8 +1342,8 @@
       <c r="L6" s="30"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" hidden="1">
-      <c r="A7" s="43"/>
-      <c r="B7" s="43"/>
+      <c r="A7" s="50"/>
+      <c r="B7" s="50"/>
       <c r="C7" s="4" t="s">
         <v>13</v>
       </c>
@@ -1344,10 +1358,10 @@
       <c r="L7" s="30"/>
     </row>
     <row r="8" spans="1:12" ht="15.75" hidden="1">
-      <c r="A8" s="43">
+      <c r="A8" s="50">
         <v>2</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="50" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -1364,8 +1378,8 @@
       <c r="L8" s="30"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" hidden="1">
-      <c r="A9" s="43"/>
-      <c r="B9" s="43"/>
+      <c r="A9" s="50"/>
+      <c r="B9" s="50"/>
       <c r="C9" s="4" t="s">
         <v>10</v>
       </c>
@@ -1380,8 +1394,8 @@
       <c r="L9" s="30"/>
     </row>
     <row r="10" spans="1:12" ht="15.75" hidden="1">
-      <c r="A10" s="43"/>
-      <c r="B10" s="43"/>
+      <c r="A10" s="50"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1396,8 +1410,8 @@
       <c r="L10" s="30"/>
     </row>
     <row r="11" spans="1:12" ht="15.75" hidden="1">
-      <c r="A11" s="43"/>
-      <c r="B11" s="43"/>
+      <c r="A11" s="50"/>
+      <c r="B11" s="50"/>
       <c r="C11" s="4" t="s">
         <v>15</v>
       </c>
@@ -1412,8 +1426,8 @@
       <c r="L11" s="30"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" hidden="1">
-      <c r="A12" s="43"/>
-      <c r="B12" s="43"/>
+      <c r="A12" s="50"/>
+      <c r="B12" s="50"/>
       <c r="C12" s="4" t="s">
         <v>14</v>
       </c>
@@ -1428,10 +1442,10 @@
       <c r="L12" s="30"/>
     </row>
     <row r="13" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A13" s="40">
+      <c r="A13" s="47">
         <v>3</v>
       </c>
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="51" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="24" t="s">
@@ -1448,8 +1462,8 @@
       <c r="L13" s="31"/>
     </row>
     <row r="14" spans="1:12" ht="15.75">
-      <c r="A14" s="41"/>
-      <c r="B14" s="45"/>
+      <c r="A14" s="48"/>
+      <c r="B14" s="52"/>
       <c r="C14" s="22" t="s">
         <v>70</v>
       </c>
@@ -1468,8 +1482,8 @@
       <c r="L14" s="31"/>
     </row>
     <row r="15" spans="1:12" ht="15.75">
-      <c r="A15" s="41"/>
-      <c r="B15" s="45"/>
+      <c r="A15" s="48"/>
+      <c r="B15" s="52"/>
       <c r="C15" s="22" t="s">
         <v>71</v>
       </c>
@@ -1488,8 +1502,8 @@
       <c r="L15" s="31"/>
     </row>
     <row r="16" spans="1:12" ht="15.75">
-      <c r="A16" s="41"/>
-      <c r="B16" s="45"/>
+      <c r="A16" s="48"/>
+      <c r="B16" s="52"/>
       <c r="C16" s="22" t="s">
         <v>72</v>
       </c>
@@ -1508,8 +1522,8 @@
       <c r="L16" s="31"/>
     </row>
     <row r="17" spans="1:12" ht="15.75">
-      <c r="A17" s="41"/>
-      <c r="B17" s="45"/>
+      <c r="A17" s="48"/>
+      <c r="B17" s="52"/>
       <c r="C17" s="23" t="s">
         <v>73</v>
       </c>
@@ -1528,8 +1542,8 @@
       <c r="L17" s="31"/>
     </row>
     <row r="18" spans="1:12" ht="15.75">
-      <c r="A18" s="41"/>
-      <c r="B18" s="45"/>
+      <c r="A18" s="48"/>
+      <c r="B18" s="52"/>
       <c r="C18" s="5" t="s">
         <v>17</v>
       </c>
@@ -1544,8 +1558,8 @@
       <c r="L18" s="31"/>
     </row>
     <row r="19" spans="1:12" ht="15.75">
-      <c r="A19" s="41"/>
-      <c r="B19" s="45"/>
+      <c r="A19" s="48"/>
+      <c r="B19" s="52"/>
       <c r="C19" s="6" t="s">
         <v>18</v>
       </c>
@@ -1562,8 +1576,8 @@
       <c r="L19" s="31"/>
     </row>
     <row r="20" spans="1:12" ht="15.75">
-      <c r="A20" s="41"/>
-      <c r="B20" s="45"/>
+      <c r="A20" s="48"/>
+      <c r="B20" s="52"/>
       <c r="C20" s="6" t="s">
         <v>74</v>
       </c>
@@ -1582,8 +1596,8 @@
       <c r="L20" s="31"/>
     </row>
     <row r="21" spans="1:12" ht="15.75">
-      <c r="A21" s="41"/>
-      <c r="B21" s="45"/>
+      <c r="A21" s="48"/>
+      <c r="B21" s="52"/>
       <c r="C21" s="7" t="s">
         <v>19</v>
       </c>
@@ -1598,8 +1612,8 @@
       <c r="L21" s="31"/>
     </row>
     <row r="22" spans="1:12" ht="15.75">
-      <c r="A22" s="41"/>
-      <c r="B22" s="45"/>
+      <c r="A22" s="48"/>
+      <c r="B22" s="52"/>
       <c r="C22" s="27" t="s">
         <v>82</v>
       </c>
@@ -1609,7 +1623,7 @@
       <c r="G22" s="30"/>
       <c r="H22" s="38"/>
       <c r="I22" s="14"/>
-      <c r="J22" s="50">
+      <c r="J22" s="40">
         <v>41680</v>
       </c>
       <c r="K22" s="14" t="s">
@@ -1618,28 +1632,28 @@
       <c r="L22" s="31"/>
     </row>
     <row r="23" spans="1:12" ht="15.75">
-      <c r="A23" s="41"/>
-      <c r="B23" s="45"/>
-      <c r="C23" s="51" t="s">
+      <c r="A23" s="48"/>
+      <c r="B23" s="52"/>
+      <c r="C23" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="52"/>
-      <c r="G23" s="52"/>
-      <c r="H23" s="53">
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="43">
         <v>2</v>
       </c>
-      <c r="I23" s="54"/>
-      <c r="J23" s="55">
-        <v>41680</v>
-      </c>
-      <c r="K23" s="54"/>
-      <c r="L23" s="52"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="45">
+        <v>41680</v>
+      </c>
+      <c r="K23" s="44"/>
+      <c r="L23" s="42"/>
     </row>
     <row r="24" spans="1:12" ht="15.75">
-      <c r="A24" s="41"/>
-      <c r="B24" s="45"/>
+      <c r="A24" s="48"/>
+      <c r="B24" s="52"/>
       <c r="C24" s="28" t="s">
         <v>84</v>
       </c>
@@ -1651,7 +1665,7 @@
       </c>
       <c r="H24" s="38"/>
       <c r="I24" s="14"/>
-      <c r="J24" s="50">
+      <c r="J24" s="40">
         <v>41680</v>
       </c>
       <c r="K24" s="14" t="s">
@@ -1660,8 +1674,8 @@
       <c r="L24" s="31"/>
     </row>
     <row r="25" spans="1:12" ht="15.75">
-      <c r="A25" s="41"/>
-      <c r="B25" s="45"/>
+      <c r="A25" s="48"/>
+      <c r="B25" s="52"/>
       <c r="C25" s="28" t="s">
         <v>85</v>
       </c>
@@ -1673,7 +1687,7 @@
       </c>
       <c r="H25" s="38"/>
       <c r="I25" s="14"/>
-      <c r="J25" s="50">
+      <c r="J25" s="40">
         <v>41680</v>
       </c>
       <c r="K25" s="14" t="s">
@@ -1682,28 +1696,28 @@
       <c r="L25" s="31"/>
     </row>
     <row r="26" spans="1:12" ht="15.75">
-      <c r="A26" s="41"/>
-      <c r="B26" s="45"/>
-      <c r="C26" s="51" t="s">
+      <c r="A26" s="48"/>
+      <c r="B26" s="52"/>
+      <c r="C26" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="D26" s="52"/>
-      <c r="E26" s="52"/>
-      <c r="F26" s="52"/>
-      <c r="G26" s="52"/>
-      <c r="H26" s="53">
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="43">
         <v>10</v>
       </c>
-      <c r="I26" s="54"/>
-      <c r="J26" s="55">
-        <v>41680</v>
-      </c>
-      <c r="K26" s="54"/>
-      <c r="L26" s="52"/>
+      <c r="I26" s="44"/>
+      <c r="J26" s="45">
+        <v>41680</v>
+      </c>
+      <c r="K26" s="44"/>
+      <c r="L26" s="42"/>
     </row>
     <row r="27" spans="1:12" ht="15.75">
-      <c r="A27" s="41"/>
-      <c r="B27" s="45"/>
+      <c r="A27" s="48"/>
+      <c r="B27" s="52"/>
       <c r="C27" s="28" t="s">
         <v>87</v>
       </c>
@@ -1715,7 +1729,7 @@
       </c>
       <c r="H27" s="38"/>
       <c r="I27" s="14"/>
-      <c r="J27" s="50">
+      <c r="J27" s="40">
         <v>41680</v>
       </c>
       <c r="K27" s="14" t="s">
@@ -1724,8 +1738,8 @@
       <c r="L27" s="31"/>
     </row>
     <row r="28" spans="1:12" ht="15.75">
-      <c r="A28" s="41"/>
-      <c r="B28" s="45"/>
+      <c r="A28" s="48"/>
+      <c r="B28" s="52"/>
       <c r="C28" s="28" t="s">
         <v>88</v>
       </c>
@@ -1737,7 +1751,7 @@
       </c>
       <c r="H28" s="38"/>
       <c r="I28" s="14"/>
-      <c r="J28" s="50">
+      <c r="J28" s="40">
         <v>41680</v>
       </c>
       <c r="K28" s="14" t="s">
@@ -1746,8 +1760,8 @@
       <c r="L28" s="31"/>
     </row>
     <row r="29" spans="1:12" ht="15.75">
-      <c r="A29" s="41"/>
-      <c r="B29" s="45"/>
+      <c r="A29" s="48"/>
+      <c r="B29" s="52"/>
       <c r="C29" s="28" t="s">
         <v>89</v>
       </c>
@@ -1759,7 +1773,7 @@
       </c>
       <c r="H29" s="38"/>
       <c r="I29" s="14"/>
-      <c r="J29" s="50">
+      <c r="J29" s="40">
         <v>41680</v>
       </c>
       <c r="K29" s="14" t="s">
@@ -1768,8 +1782,8 @@
       <c r="L29" s="31"/>
     </row>
     <row r="30" spans="1:12" ht="15.75">
-      <c r="A30" s="41"/>
-      <c r="B30" s="45"/>
+      <c r="A30" s="48"/>
+      <c r="B30" s="52"/>
       <c r="C30" s="28" t="s">
         <v>90</v>
       </c>
@@ -1781,7 +1795,7 @@
       </c>
       <c r="H30" s="38"/>
       <c r="I30" s="14"/>
-      <c r="J30" s="50">
+      <c r="J30" s="40">
         <v>41680</v>
       </c>
       <c r="K30" s="14" t="s">
@@ -1790,8 +1804,8 @@
       <c r="L30" s="31"/>
     </row>
     <row r="31" spans="1:12" ht="15.75">
-      <c r="A31" s="41"/>
-      <c r="B31" s="45"/>
+      <c r="A31" s="48"/>
+      <c r="B31" s="52"/>
       <c r="C31" s="29" t="s">
         <v>91</v>
       </c>
@@ -1803,7 +1817,7 @@
       </c>
       <c r="H31" s="38"/>
       <c r="I31" s="14"/>
-      <c r="J31" s="50">
+      <c r="J31" s="40">
         <v>41680</v>
       </c>
       <c r="K31" s="14" t="s">
@@ -1812,8 +1826,8 @@
       <c r="L31" s="32"/>
     </row>
     <row r="32" spans="1:12" ht="15.75">
-      <c r="A32" s="41"/>
-      <c r="B32" s="45"/>
+      <c r="A32" s="48"/>
+      <c r="B32" s="52"/>
       <c r="C32" s="29" t="s">
         <v>92</v>
       </c>
@@ -1825,7 +1839,7 @@
       </c>
       <c r="H32" s="38"/>
       <c r="I32" s="14"/>
-      <c r="J32" s="50">
+      <c r="J32" s="40">
         <v>41680</v>
       </c>
       <c r="K32" s="14" t="s">
@@ -1834,8 +1848,8 @@
       <c r="L32" s="32"/>
     </row>
     <row r="33" spans="1:12" ht="15.75">
-      <c r="A33" s="41"/>
-      <c r="B33" s="45"/>
+      <c r="A33" s="48"/>
+      <c r="B33" s="52"/>
       <c r="C33" s="29" t="s">
         <v>93</v>
       </c>
@@ -1846,7 +1860,7 @@
       </c>
       <c r="H33" s="38"/>
       <c r="I33" s="14"/>
-      <c r="J33" s="50">
+      <c r="J33" s="40">
         <v>41680</v>
       </c>
       <c r="K33" s="14" t="s">
@@ -1855,8 +1869,8 @@
       <c r="L33" s="32"/>
     </row>
     <row r="34" spans="1:12" ht="15.75">
-      <c r="A34" s="41"/>
-      <c r="B34" s="45"/>
+      <c r="A34" s="48"/>
+      <c r="B34" s="52"/>
       <c r="C34" s="29" t="s">
         <v>109</v>
       </c>
@@ -1868,7 +1882,7 @@
       </c>
       <c r="H34" s="38"/>
       <c r="I34" s="14"/>
-      <c r="J34" s="50">
+      <c r="J34" s="40">
         <v>41680</v>
       </c>
       <c r="K34" s="14" t="s">
@@ -1877,8 +1891,8 @@
       <c r="L34" s="32"/>
     </row>
     <row r="35" spans="1:12" ht="15.75">
-      <c r="A35" s="41"/>
-      <c r="B35" s="45"/>
+      <c r="A35" s="48"/>
+      <c r="B35" s="52"/>
       <c r="C35" s="29" t="s">
         <v>94</v>
       </c>
@@ -1890,7 +1904,7 @@
       <c r="G35" s="30"/>
       <c r="H35" s="38"/>
       <c r="I35" s="14"/>
-      <c r="J35" s="50">
+      <c r="J35" s="40">
         <v>41680</v>
       </c>
       <c r="K35" s="14" t="s">
@@ -1899,8 +1913,8 @@
       <c r="L35" s="32"/>
     </row>
     <row r="36" spans="1:12" ht="15.75">
-      <c r="A36" s="41"/>
-      <c r="B36" s="45"/>
+      <c r="A36" s="48"/>
+      <c r="B36" s="52"/>
       <c r="C36" s="29" t="s">
         <v>95</v>
       </c>
@@ -1912,7 +1926,7 @@
       <c r="G36" s="30"/>
       <c r="H36" s="38"/>
       <c r="I36" s="14"/>
-      <c r="J36" s="50">
+      <c r="J36" s="40">
         <v>41680</v>
       </c>
       <c r="K36" s="14" t="s">
@@ -1921,28 +1935,28 @@
       <c r="L36" s="32"/>
     </row>
     <row r="37" spans="1:12" ht="15.75">
-      <c r="A37" s="41"/>
-      <c r="B37" s="45"/>
-      <c r="C37" s="51" t="s">
+      <c r="A37" s="48"/>
+      <c r="B37" s="52"/>
+      <c r="C37" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="D37" s="52"/>
-      <c r="E37" s="56"/>
-      <c r="F37" s="52"/>
-      <c r="G37" s="52"/>
-      <c r="H37" s="53">
-        <v>6</v>
-      </c>
-      <c r="I37" s="54"/>
-      <c r="J37" s="55">
-        <v>41680</v>
-      </c>
-      <c r="K37" s="54"/>
-      <c r="L37" s="54"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="46"/>
+      <c r="F37" s="42"/>
+      <c r="G37" s="42"/>
+      <c r="H37" s="43">
+        <v>7</v>
+      </c>
+      <c r="I37" s="44"/>
+      <c r="J37" s="45">
+        <v>41680</v>
+      </c>
+      <c r="K37" s="44"/>
+      <c r="L37" s="44"/>
     </row>
     <row r="38" spans="1:12" ht="15.75">
-      <c r="A38" s="41"/>
-      <c r="B38" s="45"/>
+      <c r="A38" s="48"/>
+      <c r="B38" s="52"/>
       <c r="C38" s="29" t="s">
         <v>97</v>
       </c>
@@ -1954,7 +1968,7 @@
       <c r="G38" s="30"/>
       <c r="H38" s="38"/>
       <c r="I38" s="14"/>
-      <c r="J38" s="50">
+      <c r="J38" s="40">
         <v>41680</v>
       </c>
       <c r="K38" s="14" t="s">
@@ -1963,8 +1977,8 @@
       <c r="L38" s="32"/>
     </row>
     <row r="39" spans="1:12" ht="15.75">
-      <c r="A39" s="41"/>
-      <c r="B39" s="45"/>
+      <c r="A39" s="48"/>
+      <c r="B39" s="52"/>
       <c r="C39" s="29" t="s">
         <v>98</v>
       </c>
@@ -1976,7 +1990,7 @@
       <c r="G39" s="30"/>
       <c r="H39" s="38"/>
       <c r="I39" s="14"/>
-      <c r="J39" s="50">
+      <c r="J39" s="40">
         <v>41680</v>
       </c>
       <c r="K39" s="14" t="s">
@@ -1985,8 +1999,8 @@
       <c r="L39" s="32"/>
     </row>
     <row r="40" spans="1:12" ht="15.75">
-      <c r="A40" s="41"/>
-      <c r="B40" s="45"/>
+      <c r="A40" s="48"/>
+      <c r="B40" s="52"/>
       <c r="C40" s="29" t="s">
         <v>99</v>
       </c>
@@ -1998,7 +2012,7 @@
       <c r="G40" s="30"/>
       <c r="H40" s="38"/>
       <c r="I40" s="14"/>
-      <c r="J40" s="50">
+      <c r="J40" s="40">
         <v>41680</v>
       </c>
       <c r="K40" s="14" t="s">
@@ -2007,8 +2021,8 @@
       <c r="L40" s="32"/>
     </row>
     <row r="41" spans="1:12" ht="15.75">
-      <c r="A41" s="41"/>
-      <c r="B41" s="45"/>
+      <c r="A41" s="48"/>
+      <c r="B41" s="52"/>
       <c r="C41" s="29" t="s">
         <v>100</v>
       </c>
@@ -2020,7 +2034,7 @@
       <c r="G41" s="30"/>
       <c r="H41" s="38"/>
       <c r="I41" s="14"/>
-      <c r="J41" s="50">
+      <c r="J41" s="40">
         <v>41680</v>
       </c>
       <c r="K41" s="14" t="s">
@@ -2029,95 +2043,95 @@
       <c r="L41" s="32"/>
     </row>
     <row r="42" spans="1:12" ht="15.75">
-      <c r="A42" s="41"/>
-      <c r="B42" s="45"/>
-      <c r="C42" s="29" t="s">
+      <c r="A42" s="48"/>
+      <c r="B42" s="52"/>
+      <c r="C42" s="57" t="s">
         <v>101</v>
       </c>
-      <c r="D42" s="30"/>
-      <c r="E42" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="G42" s="30"/>
-      <c r="H42" s="38"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="50">
-        <v>41680</v>
-      </c>
-      <c r="K42" s="14" t="s">
+      <c r="D42" s="58"/>
+      <c r="E42" s="58" t="s">
+        <v>8</v>
+      </c>
+      <c r="G42" s="58"/>
+      <c r="H42" s="59"/>
+      <c r="I42" s="60"/>
+      <c r="J42" s="61">
+        <v>41680</v>
+      </c>
+      <c r="K42" s="60" t="s">
         <v>125</v>
       </c>
       <c r="L42" s="32"/>
     </row>
     <row r="43" spans="1:12" ht="15.75">
-      <c r="A43" s="41"/>
-      <c r="B43" s="45"/>
-      <c r="C43" s="39" t="s">
-        <v>109</v>
-      </c>
-      <c r="D43" s="30"/>
-      <c r="E43" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="F43" s="35"/>
-      <c r="G43" s="30"/>
+      <c r="A43" s="48"/>
+      <c r="B43" s="52"/>
+      <c r="C43" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="D43" s="35"/>
+      <c r="E43" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="F43" s="21"/>
+      <c r="G43" s="35"/>
       <c r="H43" s="38"/>
       <c r="I43" s="14"/>
-      <c r="J43" s="50">
-        <v>41680</v>
-      </c>
-      <c r="K43" s="14" t="s">
+      <c r="J43" s="61">
+        <v>41680</v>
+      </c>
+      <c r="K43" s="60" t="s">
         <v>125</v>
       </c>
       <c r="L43" s="32"/>
     </row>
     <row r="44" spans="1:12" ht="15.75">
-      <c r="A44" s="41"/>
-      <c r="B44" s="45"/>
-      <c r="C44" s="51" t="s">
+      <c r="A44" s="48"/>
+      <c r="B44" s="52"/>
+      <c r="C44" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="D44" s="30"/>
+      <c r="E44" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="F44" s="35"/>
+      <c r="G44" s="30"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="14"/>
+      <c r="J44" s="40">
+        <v>41680</v>
+      </c>
+      <c r="K44" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="L44" s="32"/>
+    </row>
+    <row r="45" spans="1:12" ht="15.75">
+      <c r="A45" s="48"/>
+      <c r="B45" s="52"/>
+      <c r="C45" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="D44" s="52"/>
-      <c r="E44" s="52"/>
-      <c r="F44" s="52"/>
-      <c r="G44" s="52"/>
-      <c r="H44" s="53">
+      <c r="D45" s="42"/>
+      <c r="E45" s="42"/>
+      <c r="F45" s="42"/>
+      <c r="G45" s="42"/>
+      <c r="H45" s="43">
         <v>21</v>
       </c>
-      <c r="I44" s="54"/>
-      <c r="J44" s="55">
-        <v>41680</v>
-      </c>
-      <c r="K44" s="54"/>
-      <c r="L44" s="54"/>
-    </row>
-    <row r="45" spans="1:12" ht="15.75">
-      <c r="A45" s="41"/>
-      <c r="B45" s="45"/>
-      <c r="C45" s="29" t="s">
+      <c r="I45" s="44"/>
+      <c r="J45" s="45">
+        <v>41680</v>
+      </c>
+      <c r="K45" s="44"/>
+      <c r="L45" s="44"/>
+    </row>
+    <row r="46" spans="1:12" ht="15.75">
+      <c r="A46" s="48"/>
+      <c r="B46" s="52"/>
+      <c r="C46" s="29" t="s">
         <v>103</v>
-      </c>
-      <c r="D45" s="30"/>
-      <c r="E45" s="30"/>
-      <c r="F45" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="G45" s="30"/>
-      <c r="H45" s="38"/>
-      <c r="I45" s="14"/>
-      <c r="J45" s="50">
-        <v>41680</v>
-      </c>
-      <c r="K45" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="L45" s="32"/>
-    </row>
-    <row r="46" spans="1:12" ht="15.75">
-      <c r="A46" s="41"/>
-      <c r="B46" s="45"/>
-      <c r="C46" s="29" t="s">
-        <v>104</v>
       </c>
       <c r="D46" s="30"/>
       <c r="E46" s="30"/>
@@ -2127,7 +2141,7 @@
       <c r="G46" s="30"/>
       <c r="H46" s="38"/>
       <c r="I46" s="14"/>
-      <c r="J46" s="50">
+      <c r="J46" s="40">
         <v>41680</v>
       </c>
       <c r="K46" s="14" t="s">
@@ -2136,10 +2150,10 @@
       <c r="L46" s="32"/>
     </row>
     <row r="47" spans="1:12" ht="15.75">
-      <c r="A47" s="41"/>
-      <c r="B47" s="45"/>
+      <c r="A47" s="48"/>
+      <c r="B47" s="52"/>
       <c r="C47" s="29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D47" s="30"/>
       <c r="E47" s="30"/>
@@ -2149,7 +2163,7 @@
       <c r="G47" s="30"/>
       <c r="H47" s="38"/>
       <c r="I47" s="14"/>
-      <c r="J47" s="50">
+      <c r="J47" s="40">
         <v>41680</v>
       </c>
       <c r="K47" s="14" t="s">
@@ -2158,10 +2172,10 @@
       <c r="L47" s="32"/>
     </row>
     <row r="48" spans="1:12" ht="15.75">
-      <c r="A48" s="41"/>
-      <c r="B48" s="45"/>
+      <c r="A48" s="48"/>
+      <c r="B48" s="52"/>
       <c r="C48" s="29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D48" s="30"/>
       <c r="E48" s="30"/>
@@ -2171,7 +2185,7 @@
       <c r="G48" s="30"/>
       <c r="H48" s="38"/>
       <c r="I48" s="14"/>
-      <c r="J48" s="50">
+      <c r="J48" s="40">
         <v>41680</v>
       </c>
       <c r="K48" s="14" t="s">
@@ -2180,10 +2194,10 @@
       <c r="L48" s="32"/>
     </row>
     <row r="49" spans="1:12" ht="15.75">
-      <c r="A49" s="41"/>
-      <c r="B49" s="45"/>
+      <c r="A49" s="48"/>
+      <c r="B49" s="52"/>
       <c r="C49" s="29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D49" s="30"/>
       <c r="E49" s="30"/>
@@ -2193,7 +2207,7 @@
       <c r="G49" s="30"/>
       <c r="H49" s="38"/>
       <c r="I49" s="14"/>
-      <c r="J49" s="50">
+      <c r="J49" s="40">
         <v>41680</v>
       </c>
       <c r="K49" s="14" t="s">
@@ -2202,10 +2216,10 @@
       <c r="L49" s="32"/>
     </row>
     <row r="50" spans="1:12" ht="15.75">
-      <c r="A50" s="41"/>
-      <c r="B50" s="45"/>
+      <c r="A50" s="48"/>
+      <c r="B50" s="52"/>
       <c r="C50" s="29" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D50" s="30"/>
       <c r="E50" s="30"/>
@@ -2215,7 +2229,7 @@
       <c r="G50" s="30"/>
       <c r="H50" s="38"/>
       <c r="I50" s="14"/>
-      <c r="J50" s="50">
+      <c r="J50" s="40">
         <v>41680</v>
       </c>
       <c r="K50" s="14" t="s">
@@ -2224,10 +2238,10 @@
       <c r="L50" s="32"/>
     </row>
     <row r="51" spans="1:12" ht="15.75">
-      <c r="A51" s="41"/>
-      <c r="B51" s="45"/>
+      <c r="A51" s="48"/>
+      <c r="B51" s="52"/>
       <c r="C51" s="29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D51" s="30"/>
       <c r="E51" s="30"/>
@@ -2237,7 +2251,7 @@
       <c r="G51" s="30"/>
       <c r="H51" s="38"/>
       <c r="I51" s="14"/>
-      <c r="J51" s="50">
+      <c r="J51" s="40">
         <v>41680</v>
       </c>
       <c r="K51" s="14" t="s">
@@ -2246,20 +2260,20 @@
       <c r="L51" s="32"/>
     </row>
     <row r="52" spans="1:12" ht="15.75">
-      <c r="A52" s="41"/>
-      <c r="B52" s="45"/>
+      <c r="A52" s="48"/>
+      <c r="B52" s="52"/>
       <c r="C52" s="29" t="s">
-        <v>110</v>
-      </c>
-      <c r="D52" s="30" t="s">
-        <v>8</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="D52" s="30"/>
       <c r="E52" s="30"/>
-      <c r="F52" s="30"/>
+      <c r="F52" s="30" t="s">
+        <v>8</v>
+      </c>
       <c r="G52" s="30"/>
       <c r="H52" s="38"/>
       <c r="I52" s="14"/>
-      <c r="J52" s="50">
+      <c r="J52" s="40">
         <v>41680</v>
       </c>
       <c r="K52" s="14" t="s">
@@ -2268,10 +2282,10 @@
       <c r="L52" s="32"/>
     </row>
     <row r="53" spans="1:12" ht="15.75">
-      <c r="A53" s="41"/>
-      <c r="B53" s="45"/>
+      <c r="A53" s="48"/>
+      <c r="B53" s="52"/>
       <c r="C53" s="29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D53" s="30" t="s">
         <v>8</v>
@@ -2281,7 +2295,7 @@
       <c r="G53" s="30"/>
       <c r="H53" s="38"/>
       <c r="I53" s="14"/>
-      <c r="J53" s="50">
+      <c r="J53" s="40">
         <v>41680</v>
       </c>
       <c r="K53" s="14" t="s">
@@ -2290,10 +2304,10 @@
       <c r="L53" s="32"/>
     </row>
     <row r="54" spans="1:12" ht="15.75">
-      <c r="A54" s="41"/>
-      <c r="B54" s="45"/>
+      <c r="A54" s="48"/>
+      <c r="B54" s="52"/>
       <c r="C54" s="29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D54" s="30" t="s">
         <v>8</v>
@@ -2303,7 +2317,7 @@
       <c r="G54" s="30"/>
       <c r="H54" s="38"/>
       <c r="I54" s="14"/>
-      <c r="J54" s="50">
+      <c r="J54" s="40">
         <v>41680</v>
       </c>
       <c r="K54" s="14" t="s">
@@ -2312,10 +2326,10 @@
       <c r="L54" s="32"/>
     </row>
     <row r="55" spans="1:12" ht="15.75">
-      <c r="A55" s="41"/>
-      <c r="B55" s="45"/>
+      <c r="A55" s="48"/>
+      <c r="B55" s="52"/>
       <c r="C55" s="29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D55" s="30" t="s">
         <v>8</v>
@@ -2325,7 +2339,7 @@
       <c r="G55" s="30"/>
       <c r="H55" s="38"/>
       <c r="I55" s="14"/>
-      <c r="J55" s="50">
+      <c r="J55" s="40">
         <v>41680</v>
       </c>
       <c r="K55" s="14" t="s">
@@ -2334,10 +2348,10 @@
       <c r="L55" s="32"/>
     </row>
     <row r="56" spans="1:12" ht="15.75">
-      <c r="A56" s="41"/>
-      <c r="B56" s="45"/>
+      <c r="A56" s="48"/>
+      <c r="B56" s="52"/>
       <c r="C56" s="29" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D56" s="30" t="s">
         <v>8</v>
@@ -2347,7 +2361,7 @@
       <c r="G56" s="30"/>
       <c r="H56" s="38"/>
       <c r="I56" s="14"/>
-      <c r="J56" s="50">
+      <c r="J56" s="40">
         <v>41680</v>
       </c>
       <c r="K56" s="14" t="s">
@@ -2356,10 +2370,10 @@
       <c r="L56" s="32"/>
     </row>
     <row r="57" spans="1:12" ht="15.75">
-      <c r="A57" s="41"/>
-      <c r="B57" s="45"/>
+      <c r="A57" s="48"/>
+      <c r="B57" s="52"/>
       <c r="C57" s="29" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D57" s="30" t="s">
         <v>8</v>
@@ -2369,7 +2383,7 @@
       <c r="G57" s="30"/>
       <c r="H57" s="38"/>
       <c r="I57" s="14"/>
-      <c r="J57" s="50">
+      <c r="J57" s="40">
         <v>41680</v>
       </c>
       <c r="K57" s="14" t="s">
@@ -2378,10 +2392,10 @@
       <c r="L57" s="32"/>
     </row>
     <row r="58" spans="1:12" ht="15.75">
-      <c r="A58" s="41"/>
-      <c r="B58" s="45"/>
+      <c r="A58" s="48"/>
+      <c r="B58" s="52"/>
       <c r="C58" s="29" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D58" s="30" t="s">
         <v>8</v>
@@ -2391,7 +2405,7 @@
       <c r="G58" s="30"/>
       <c r="H58" s="38"/>
       <c r="I58" s="14"/>
-      <c r="J58" s="50">
+      <c r="J58" s="40">
         <v>41680</v>
       </c>
       <c r="K58" s="14" t="s">
@@ -2400,10 +2414,10 @@
       <c r="L58" s="32"/>
     </row>
     <row r="59" spans="1:12" ht="15.75">
-      <c r="A59" s="41"/>
-      <c r="B59" s="45"/>
+      <c r="A59" s="48"/>
+      <c r="B59" s="52"/>
       <c r="C59" s="29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D59" s="30" t="s">
         <v>8</v>
@@ -2413,7 +2427,7 @@
       <c r="G59" s="30"/>
       <c r="H59" s="38"/>
       <c r="I59" s="14"/>
-      <c r="J59" s="50">
+      <c r="J59" s="40">
         <v>41680</v>
       </c>
       <c r="K59" s="14" t="s">
@@ -2422,10 +2436,10 @@
       <c r="L59" s="32"/>
     </row>
     <row r="60" spans="1:12" ht="15.75">
-      <c r="A60" s="41"/>
-      <c r="B60" s="45"/>
+      <c r="A60" s="48"/>
+      <c r="B60" s="52"/>
       <c r="C60" s="29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D60" s="30" t="s">
         <v>8</v>
@@ -2435,7 +2449,7 @@
       <c r="G60" s="30"/>
       <c r="H60" s="38"/>
       <c r="I60" s="14"/>
-      <c r="J60" s="50">
+      <c r="J60" s="40">
         <v>41680</v>
       </c>
       <c r="K60" s="14" t="s">
@@ -2444,10 +2458,10 @@
       <c r="L60" s="32"/>
     </row>
     <row r="61" spans="1:12" ht="15.75">
-      <c r="A61" s="41"/>
-      <c r="B61" s="45"/>
+      <c r="A61" s="48"/>
+      <c r="B61" s="52"/>
       <c r="C61" s="29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D61" s="30" t="s">
         <v>8</v>
@@ -2457,7 +2471,7 @@
       <c r="G61" s="30"/>
       <c r="H61" s="38"/>
       <c r="I61" s="14"/>
-      <c r="J61" s="50">
+      <c r="J61" s="40">
         <v>41680</v>
       </c>
       <c r="K61" s="14" t="s">
@@ -2466,10 +2480,10 @@
       <c r="L61" s="32"/>
     </row>
     <row r="62" spans="1:12" ht="15.75">
-      <c r="A62" s="41"/>
-      <c r="B62" s="45"/>
+      <c r="A62" s="48"/>
+      <c r="B62" s="52"/>
       <c r="C62" s="29" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D62" s="30" t="s">
         <v>8</v>
@@ -2479,7 +2493,7 @@
       <c r="G62" s="30"/>
       <c r="H62" s="38"/>
       <c r="I62" s="14"/>
-      <c r="J62" s="50">
+      <c r="J62" s="40">
         <v>41680</v>
       </c>
       <c r="K62" s="14" t="s">
@@ -2488,20 +2502,20 @@
       <c r="L62" s="32"/>
     </row>
     <row r="63" spans="1:12" ht="15.75">
-      <c r="A63" s="41"/>
-      <c r="B63" s="45"/>
+      <c r="A63" s="48"/>
+      <c r="B63" s="52"/>
       <c r="C63" s="29" t="s">
-        <v>121</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
-      <c r="G63" s="2"/>
+        <v>120</v>
+      </c>
+      <c r="D63" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E63" s="30"/>
+      <c r="F63" s="30"/>
+      <c r="G63" s="30"/>
       <c r="H63" s="38"/>
       <c r="I63" s="14"/>
-      <c r="J63" s="50">
+      <c r="J63" s="40">
         <v>41680</v>
       </c>
       <c r="K63" s="14" t="s">
@@ -2510,20 +2524,20 @@
       <c r="L63" s="32"/>
     </row>
     <row r="64" spans="1:12" ht="15.75">
-      <c r="A64" s="41"/>
-      <c r="B64" s="45"/>
+      <c r="A64" s="48"/>
+      <c r="B64" s="52"/>
       <c r="C64" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="D64" s="2"/>
-      <c r="E64" s="2" t="s">
-        <v>8</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E64" s="2"/>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
       <c r="H64" s="38"/>
       <c r="I64" s="14"/>
-      <c r="J64" s="50">
+      <c r="J64" s="40">
         <v>41680</v>
       </c>
       <c r="K64" s="14" t="s">
@@ -2532,10 +2546,10 @@
       <c r="L64" s="32"/>
     </row>
     <row r="65" spans="1:12" ht="15.75">
-      <c r="A65" s="41"/>
-      <c r="B65" s="45"/>
+      <c r="A65" s="48"/>
+      <c r="B65" s="52"/>
       <c r="C65" s="29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="2" t="s">
@@ -2545,7 +2559,7 @@
       <c r="G65" s="2"/>
       <c r="H65" s="38"/>
       <c r="I65" s="14"/>
-      <c r="J65" s="50">
+      <c r="J65" s="40">
         <v>41680</v>
       </c>
       <c r="K65" s="14" t="s">
@@ -2554,26 +2568,32 @@
       <c r="L65" s="32"/>
     </row>
     <row r="66" spans="1:12" ht="15.75">
-      <c r="A66" s="41"/>
-      <c r="B66" s="45"/>
-      <c r="C66" s="7" t="s">
-        <v>21</v>
+      <c r="A66" s="48"/>
+      <c r="B66" s="52"/>
+      <c r="C66" s="29" t="s">
+        <v>123</v>
       </c>
       <c r="D66" s="2"/>
-      <c r="E66" s="2"/>
+      <c r="E66" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
       <c r="H66" s="38"/>
       <c r="I66" s="14"/>
-      <c r="J66" s="14"/>
-      <c r="K66" s="14"/>
+      <c r="J66" s="40">
+        <v>41680</v>
+      </c>
+      <c r="K66" s="14" t="s">
+        <v>125</v>
+      </c>
       <c r="L66" s="32"/>
     </row>
     <row r="67" spans="1:12" ht="15.75">
-      <c r="A67" s="41"/>
-      <c r="B67" s="45"/>
-      <c r="C67" s="8" t="s">
-        <v>22</v>
+      <c r="A67" s="48"/>
+      <c r="B67" s="52"/>
+      <c r="C67" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
@@ -2586,10 +2606,10 @@
       <c r="L67" s="32"/>
     </row>
     <row r="68" spans="1:12" ht="15.75">
-      <c r="A68" s="42"/>
-      <c r="B68" s="46"/>
+      <c r="A68" s="48"/>
+      <c r="B68" s="52"/>
       <c r="C68" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
@@ -2602,14 +2622,10 @@
       <c r="L68" s="32"/>
     </row>
     <row r="69" spans="1:12" ht="15.75">
-      <c r="A69" s="40">
-        <v>4</v>
-      </c>
-      <c r="B69" s="40" t="s">
-        <v>6</v>
-      </c>
+      <c r="A69" s="49"/>
+      <c r="B69" s="53"/>
       <c r="C69" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
@@ -2622,10 +2638,14 @@
       <c r="L69" s="32"/>
     </row>
     <row r="70" spans="1:12" ht="15.75">
-      <c r="A70" s="41"/>
-      <c r="B70" s="41"/>
-      <c r="C70" s="9" t="s">
-        <v>25</v>
+      <c r="A70" s="47">
+        <v>4</v>
+      </c>
+      <c r="B70" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="C70" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
@@ -2638,10 +2658,10 @@
       <c r="L70" s="32"/>
     </row>
     <row r="71" spans="1:12" ht="15.75">
-      <c r="A71" s="41"/>
-      <c r="B71" s="41"/>
-      <c r="C71" s="4" t="s">
-        <v>26</v>
+      <c r="A71" s="48"/>
+      <c r="B71" s="48"/>
+      <c r="C71" s="9" t="s">
+        <v>25</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
@@ -2654,10 +2674,10 @@
       <c r="L71" s="32"/>
     </row>
     <row r="72" spans="1:12" ht="15.75">
-      <c r="A72" s="41"/>
-      <c r="B72" s="41"/>
+      <c r="A72" s="48"/>
+      <c r="B72" s="48"/>
       <c r="C72" s="4" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
@@ -2670,10 +2690,10 @@
       <c r="L72" s="32"/>
     </row>
     <row r="73" spans="1:12" ht="15.75">
-      <c r="A73" s="41"/>
-      <c r="B73" s="41"/>
-      <c r="C73" s="10" t="s">
-        <v>54</v>
+      <c r="A73" s="48"/>
+      <c r="B73" s="48"/>
+      <c r="C73" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
@@ -2686,10 +2706,10 @@
       <c r="L73" s="32"/>
     </row>
     <row r="74" spans="1:12" ht="15.75">
-      <c r="A74" s="41"/>
-      <c r="B74" s="41"/>
-      <c r="C74" s="11" t="s">
-        <v>55</v>
+      <c r="A74" s="48"/>
+      <c r="B74" s="48"/>
+      <c r="C74" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
@@ -2702,10 +2722,10 @@
       <c r="L74" s="32"/>
     </row>
     <row r="75" spans="1:12" ht="15.75">
-      <c r="A75" s="41"/>
-      <c r="B75" s="41"/>
+      <c r="A75" s="48"/>
+      <c r="B75" s="48"/>
       <c r="C75" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
@@ -2718,10 +2738,10 @@
       <c r="L75" s="32"/>
     </row>
     <row r="76" spans="1:12" ht="15.75">
-      <c r="A76" s="41"/>
-      <c r="B76" s="41"/>
-      <c r="C76" s="12" t="s">
-        <v>27</v>
+      <c r="A76" s="48"/>
+      <c r="B76" s="48"/>
+      <c r="C76" s="11" t="s">
+        <v>56</v>
       </c>
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
@@ -2734,10 +2754,10 @@
       <c r="L76" s="32"/>
     </row>
     <row r="77" spans="1:12" ht="15.75">
-      <c r="A77" s="41"/>
-      <c r="B77" s="41"/>
-      <c r="C77" s="10" t="s">
-        <v>28</v>
+      <c r="A77" s="48"/>
+      <c r="B77" s="48"/>
+      <c r="C77" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
@@ -2750,10 +2770,10 @@
       <c r="L77" s="32"/>
     </row>
     <row r="78" spans="1:12" ht="15.75">
-      <c r="A78" s="41"/>
-      <c r="B78" s="41"/>
-      <c r="C78" s="11" t="s">
-        <v>29</v>
+      <c r="A78" s="48"/>
+      <c r="B78" s="48"/>
+      <c r="C78" s="10" t="s">
+        <v>28</v>
       </c>
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
@@ -2765,11 +2785,11 @@
       <c r="K78" s="14"/>
       <c r="L78" s="32"/>
     </row>
-    <row r="79" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A79" s="41"/>
-      <c r="B79" s="41"/>
+    <row r="79" spans="1:12" ht="15.75">
+      <c r="A79" s="48"/>
+      <c r="B79" s="48"/>
       <c r="C79" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
@@ -2781,11 +2801,11 @@
       <c r="K79" s="14"/>
       <c r="L79" s="32"/>
     </row>
-    <row r="80" spans="1:12" ht="15.75">
-      <c r="A80" s="41"/>
-      <c r="B80" s="41"/>
-      <c r="C80" s="13" t="s">
-        <v>31</v>
+    <row r="80" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A80" s="48"/>
+      <c r="B80" s="48"/>
+      <c r="C80" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="D80" s="2"/>
       <c r="E80" s="2"/>
@@ -2798,10 +2818,10 @@
       <c r="L80" s="32"/>
     </row>
     <row r="81" spans="1:12" ht="15.75">
-      <c r="A81" s="41"/>
-      <c r="B81" s="41"/>
-      <c r="C81" s="8" t="s">
-        <v>50</v>
+      <c r="A81" s="48"/>
+      <c r="B81" s="48"/>
+      <c r="C81" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
@@ -2814,10 +2834,10 @@
       <c r="L81" s="32"/>
     </row>
     <row r="82" spans="1:12" ht="15.75">
-      <c r="A82" s="41"/>
-      <c r="B82" s="41"/>
+      <c r="A82" s="48"/>
+      <c r="B82" s="48"/>
       <c r="C82" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
@@ -2830,10 +2850,10 @@
       <c r="L82" s="32"/>
     </row>
     <row r="83" spans="1:12" ht="15.75">
-      <c r="A83" s="42"/>
-      <c r="B83" s="42"/>
+      <c r="A83" s="48"/>
+      <c r="B83" s="48"/>
       <c r="C83" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
@@ -2846,14 +2866,10 @@
       <c r="L83" s="32"/>
     </row>
     <row r="84" spans="1:12" ht="15.75">
-      <c r="A84" s="47">
-        <v>5</v>
-      </c>
-      <c r="B84" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="C84" s="13" t="s">
-        <v>48</v>
+      <c r="A84" s="49"/>
+      <c r="B84" s="49"/>
+      <c r="C84" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="D84" s="2"/>
       <c r="E84" s="2"/>
@@ -2866,10 +2882,14 @@
       <c r="L84" s="32"/>
     </row>
     <row r="85" spans="1:12" ht="15.75">
-      <c r="A85" s="48"/>
-      <c r="B85" s="41"/>
+      <c r="A85" s="54">
+        <v>5</v>
+      </c>
+      <c r="B85" s="47" t="s">
+        <v>58</v>
+      </c>
       <c r="C85" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D85" s="2"/>
       <c r="E85" s="2"/>
@@ -2882,10 +2902,10 @@
       <c r="L85" s="32"/>
     </row>
     <row r="86" spans="1:12" ht="15.75">
-      <c r="A86" s="48"/>
-      <c r="B86" s="41"/>
-      <c r="C86" s="5" t="s">
-        <v>40</v>
+      <c r="A86" s="55"/>
+      <c r="B86" s="48"/>
+      <c r="C86" s="13" t="s">
+        <v>49</v>
       </c>
       <c r="D86" s="2"/>
       <c r="E86" s="2"/>
@@ -2898,10 +2918,10 @@
       <c r="L86" s="32"/>
     </row>
     <row r="87" spans="1:12" ht="15.75">
-      <c r="A87" s="48"/>
-      <c r="B87" s="41"/>
+      <c r="A87" s="55"/>
+      <c r="B87" s="48"/>
       <c r="C87" s="5" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D87" s="2"/>
       <c r="E87" s="2"/>
@@ -2914,10 +2934,10 @@
       <c r="L87" s="32"/>
     </row>
     <row r="88" spans="1:12" ht="15.75">
-      <c r="A88" s="48"/>
-      <c r="B88" s="41"/>
-      <c r="C88" s="11" t="s">
-        <v>34</v>
+      <c r="A88" s="55"/>
+      <c r="B88" s="48"/>
+      <c r="C88" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="D88" s="2"/>
       <c r="E88" s="2"/>
@@ -2930,10 +2950,10 @@
       <c r="L88" s="32"/>
     </row>
     <row r="89" spans="1:12" ht="15.75">
-      <c r="A89" s="48"/>
-      <c r="B89" s="41"/>
+      <c r="A89" s="55"/>
+      <c r="B89" s="48"/>
       <c r="C89" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D89" s="2"/>
       <c r="E89" s="2"/>
@@ -2946,10 +2966,10 @@
       <c r="L89" s="32"/>
     </row>
     <row r="90" spans="1:12" ht="15.75">
-      <c r="A90" s="48"/>
-      <c r="B90" s="41"/>
-      <c r="C90" s="5" t="s">
-        <v>33</v>
+      <c r="A90" s="55"/>
+      <c r="B90" s="48"/>
+      <c r="C90" s="11" t="s">
+        <v>35</v>
       </c>
       <c r="D90" s="2"/>
       <c r="E90" s="2"/>
@@ -2962,10 +2982,10 @@
       <c r="L90" s="32"/>
     </row>
     <row r="91" spans="1:12" ht="15.75">
-      <c r="A91" s="48"/>
-      <c r="B91" s="41"/>
-      <c r="C91" s="11" t="s">
-        <v>34</v>
+      <c r="A91" s="55"/>
+      <c r="B91" s="48"/>
+      <c r="C91" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="D91" s="2"/>
       <c r="E91" s="2"/>
@@ -2978,10 +2998,10 @@
       <c r="L91" s="32"/>
     </row>
     <row r="92" spans="1:12" ht="15.75">
-      <c r="A92" s="48"/>
-      <c r="B92" s="41"/>
+      <c r="A92" s="55"/>
+      <c r="B92" s="48"/>
       <c r="C92" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D92" s="2"/>
       <c r="E92" s="2"/>
@@ -2994,10 +3014,10 @@
       <c r="L92" s="32"/>
     </row>
     <row r="93" spans="1:12" ht="15.75">
-      <c r="A93" s="48"/>
-      <c r="B93" s="41"/>
-      <c r="C93" s="4" t="s">
-        <v>59</v>
+      <c r="A93" s="55"/>
+      <c r="B93" s="48"/>
+      <c r="C93" s="11" t="s">
+        <v>35</v>
       </c>
       <c r="D93" s="2"/>
       <c r="E93" s="2"/>
@@ -3009,11 +3029,11 @@
       <c r="K93" s="14"/>
       <c r="L93" s="32"/>
     </row>
-    <row r="94" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A94" s="48"/>
-      <c r="B94" s="41"/>
-      <c r="C94" s="13" t="s">
-        <v>36</v>
+    <row r="94" spans="1:12" ht="15.75">
+      <c r="A94" s="55"/>
+      <c r="B94" s="48"/>
+      <c r="C94" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
@@ -3025,11 +3045,11 @@
       <c r="K94" s="14"/>
       <c r="L94" s="32"/>
     </row>
-    <row r="95" spans="1:12" ht="15.75">
-      <c r="A95" s="48"/>
-      <c r="B95" s="41"/>
-      <c r="C95" s="11" t="s">
-        <v>20</v>
+    <row r="95" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A95" s="55"/>
+      <c r="B95" s="48"/>
+      <c r="C95" s="13" t="s">
+        <v>36</v>
       </c>
       <c r="D95" s="2"/>
       <c r="E95" s="2"/>
@@ -3042,10 +3062,10 @@
       <c r="L95" s="32"/>
     </row>
     <row r="96" spans="1:12" ht="15.75">
-      <c r="A96" s="48"/>
-      <c r="B96" s="41"/>
+      <c r="A96" s="55"/>
+      <c r="B96" s="48"/>
       <c r="C96" s="11" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="D96" s="2"/>
       <c r="E96" s="2"/>
@@ -3058,10 +3078,10 @@
       <c r="L96" s="32"/>
     </row>
     <row r="97" spans="1:12" ht="15.75">
-      <c r="A97" s="48"/>
-      <c r="B97" s="41"/>
+      <c r="A97" s="55"/>
+      <c r="B97" s="48"/>
       <c r="C97" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D97" s="2"/>
       <c r="E97" s="2"/>
@@ -3074,10 +3094,10 @@
       <c r="L97" s="32"/>
     </row>
     <row r="98" spans="1:12" ht="15.75">
-      <c r="A98" s="48"/>
-      <c r="B98" s="41"/>
-      <c r="C98" s="13" t="s">
-        <v>37</v>
+      <c r="A98" s="55"/>
+      <c r="B98" s="48"/>
+      <c r="C98" s="11" t="s">
+        <v>39</v>
       </c>
       <c r="D98" s="2"/>
       <c r="E98" s="2"/>
@@ -3090,10 +3110,10 @@
       <c r="L98" s="32"/>
     </row>
     <row r="99" spans="1:12" ht="15.75">
-      <c r="A99" s="48"/>
-      <c r="B99" s="41"/>
-      <c r="C99" s="11" t="s">
-        <v>20</v>
+      <c r="A99" s="55"/>
+      <c r="B99" s="48"/>
+      <c r="C99" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="D99" s="2"/>
       <c r="E99" s="2"/>
@@ -3106,10 +3126,10 @@
       <c r="L99" s="32"/>
     </row>
     <row r="100" spans="1:12" ht="15.75">
-      <c r="A100" s="48"/>
-      <c r="B100" s="41"/>
+      <c r="A100" s="55"/>
+      <c r="B100" s="48"/>
       <c r="C100" s="11" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="D100" s="2"/>
       <c r="E100" s="2"/>
@@ -3122,10 +3142,10 @@
       <c r="L100" s="32"/>
     </row>
     <row r="101" spans="1:12" ht="15.75">
-      <c r="A101" s="49"/>
-      <c r="B101" s="42"/>
-      <c r="C101" s="13" t="s">
-        <v>57</v>
+      <c r="A101" s="55"/>
+      <c r="B101" s="48"/>
+      <c r="C101" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
@@ -3138,14 +3158,10 @@
       <c r="L101" s="32"/>
     </row>
     <row r="102" spans="1:12" ht="15.75">
-      <c r="A102" s="47">
-        <v>6</v>
-      </c>
-      <c r="B102" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="C102" s="11" t="s">
-        <v>20</v>
+      <c r="A102" s="56"/>
+      <c r="B102" s="49"/>
+      <c r="C102" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
@@ -3158,10 +3174,14 @@
       <c r="L102" s="32"/>
     </row>
     <row r="103" spans="1:12" ht="15.75">
-      <c r="A103" s="48"/>
-      <c r="B103" s="41"/>
+      <c r="A103" s="54">
+        <v>6</v>
+      </c>
+      <c r="B103" s="47" t="s">
+        <v>7</v>
+      </c>
       <c r="C103" s="11" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
@@ -3174,10 +3194,10 @@
       <c r="L103" s="32"/>
     </row>
     <row r="104" spans="1:12" ht="15.75">
-      <c r="A104" s="48"/>
-      <c r="B104" s="41"/>
-      <c r="C104" s="13" t="s">
-        <v>41</v>
+      <c r="A104" s="55"/>
+      <c r="B104" s="48"/>
+      <c r="C104" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="D104" s="2"/>
       <c r="E104" s="2"/>
@@ -3190,10 +3210,10 @@
       <c r="L104" s="32"/>
     </row>
     <row r="105" spans="1:12" ht="15.75">
-      <c r="A105" s="48"/>
-      <c r="B105" s="41"/>
+      <c r="A105" s="55"/>
+      <c r="B105" s="48"/>
       <c r="C105" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D105" s="2"/>
       <c r="E105" s="2"/>
@@ -3206,10 +3226,10 @@
       <c r="L105" s="32"/>
     </row>
     <row r="106" spans="1:12" ht="15.75">
-      <c r="A106" s="48"/>
-      <c r="B106" s="41"/>
-      <c r="C106" s="11" t="s">
-        <v>20</v>
+      <c r="A106" s="55"/>
+      <c r="B106" s="48"/>
+      <c r="C106" s="13" t="s">
+        <v>42</v>
       </c>
       <c r="D106" s="2"/>
       <c r="E106" s="2"/>
@@ -3222,10 +3242,10 @@
       <c r="L106" s="32"/>
     </row>
     <row r="107" spans="1:12" ht="15.75">
-      <c r="A107" s="49"/>
-      <c r="B107" s="42"/>
+      <c r="A107" s="55"/>
+      <c r="B107" s="48"/>
       <c r="C107" s="11" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="D107" s="2"/>
       <c r="E107" s="2"/>
@@ -3237,28 +3257,27 @@
       <c r="K107" s="14"/>
       <c r="L107" s="32"/>
     </row>
-    <row r="108" spans="1:12">
-      <c r="A108" s="3"/>
-      <c r="B108" s="3"/>
+    <row r="108" spans="1:12" ht="15.75">
+      <c r="A108" s="56"/>
+      <c r="B108" s="49"/>
       <c r="C108" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D108" s="2"/>
+      <c r="E108" s="2"/>
+      <c r="F108" s="2"/>
+      <c r="G108" s="2"/>
+      <c r="H108" s="38"/>
+      <c r="I108" s="14"/>
+      <c r="J108" s="14"/>
+      <c r="K108" s="14"/>
+      <c r="L108" s="32"/>
+    </row>
+    <row r="109" spans="1:12">
+      <c r="A109" s="3"/>
+      <c r="B109" s="3"/>
+      <c r="C109" s="11" t="s">
         <v>39</v>
-      </c>
-      <c r="D108" s="3"/>
-      <c r="E108" s="3"/>
-      <c r="F108" s="3"/>
-      <c r="G108" s="3"/>
-      <c r="I108" s="3"/>
-      <c r="J108" s="3"/>
-      <c r="K108" s="3"/>
-      <c r="L108" s="34"/>
-    </row>
-    <row r="109" spans="1:12">
-      <c r="A109" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="B109" s="3"/>
-      <c r="C109" s="13" t="s">
-        <v>43</v>
       </c>
       <c r="D109" s="3"/>
       <c r="E109" s="3"/>
@@ -3270,13 +3289,13 @@
       <c r="L109" s="34"/>
     </row>
     <row r="110" spans="1:12">
-      <c r="A110" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B110" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="C110" s="1"/>
+      <c r="A110" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B110" s="3"/>
+      <c r="C110" s="13" t="s">
+        <v>43</v>
+      </c>
       <c r="D110" s="3"/>
       <c r="E110" s="3"/>
       <c r="F110" s="3"/>
@@ -3286,12 +3305,12 @@
       <c r="K110" s="3"/>
       <c r="L110" s="34"/>
     </row>
-    <row r="111" spans="1:12" ht="60">
-      <c r="A111" s="19">
-        <v>1</v>
-      </c>
-      <c r="B111" s="20" t="s">
-        <v>67</v>
+    <row r="111" spans="1:12">
+      <c r="A111" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B111" s="19" t="s">
+        <v>63</v>
       </c>
       <c r="C111" s="1"/>
       <c r="D111" s="3"/>
@@ -3303,16 +3322,14 @@
       <c r="K111" s="3"/>
       <c r="L111" s="34"/>
     </row>
-    <row r="112" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A112" s="21">
-        <v>2</v>
+    <row r="112" spans="1:12" ht="60">
+      <c r="A112" s="19">
+        <v>1</v>
       </c>
       <c r="B112" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="C112" s="4" t="s">
-        <v>64</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="C112" s="1"/>
       <c r="D112" s="3"/>
       <c r="E112" s="3"/>
       <c r="F112" s="3"/>
@@ -3322,15 +3339,15 @@
       <c r="K112" s="3"/>
       <c r="L112" s="34"/>
     </row>
-    <row r="113" spans="1:12" ht="30">
+    <row r="113" spans="1:12" ht="15.75" customHeight="1">
       <c r="A113" s="21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B113" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="C113" s="4">
-        <v>1</v>
+        <v>65</v>
+      </c>
+      <c r="C113" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="D113" s="3"/>
       <c r="E113" s="3"/>
@@ -3343,13 +3360,13 @@
     </row>
     <row r="114" spans="1:12" ht="30">
       <c r="A114" s="21">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B114" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="C114" s="21">
-        <v>2</v>
+        <v>66</v>
+      </c>
+      <c r="C114" s="4">
+        <v>1</v>
       </c>
       <c r="D114" s="3"/>
       <c r="E114" s="3"/>
@@ -3362,13 +3379,13 @@
     </row>
     <row r="115" spans="1:12" ht="30">
       <c r="A115" s="21">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B115" s="20" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C115" s="21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D115" s="3"/>
       <c r="E115" s="3"/>
@@ -3379,33 +3396,52 @@
       <c r="K115" s="3"/>
       <c r="L115" s="34"/>
     </row>
-    <row r="116" spans="1:12">
+    <row r="116" spans="1:12" ht="30">
+      <c r="A116" s="21">
+        <v>5</v>
+      </c>
+      <c r="B116" s="20" t="s">
+        <v>68</v>
+      </c>
       <c r="C116" s="21">
-        <v>4</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="D116" s="3"/>
+      <c r="E116" s="3"/>
+      <c r="F116" s="3"/>
+      <c r="G116" s="3"/>
+      <c r="I116" s="3"/>
+      <c r="J116" s="3"/>
+      <c r="K116" s="3"/>
+      <c r="L116" s="34"/>
     </row>
     <row r="117" spans="1:12">
       <c r="C117" s="21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12">
+      <c r="C118" s="21">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B69:B83"/>
-    <mergeCell ref="B84:B101"/>
-    <mergeCell ref="B102:B107"/>
+    <mergeCell ref="B70:B84"/>
+    <mergeCell ref="B85:B102"/>
+    <mergeCell ref="B103:B108"/>
     <mergeCell ref="B2:B7"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="B8:B12"/>
     <mergeCell ref="A8:A12"/>
-    <mergeCell ref="A13:A68"/>
-    <mergeCell ref="B13:B68"/>
-    <mergeCell ref="A69:A83"/>
-    <mergeCell ref="A84:A101"/>
-    <mergeCell ref="A102:A107"/>
+    <mergeCell ref="A13:A69"/>
+    <mergeCell ref="B13:B69"/>
+    <mergeCell ref="A70:A84"/>
+    <mergeCell ref="A85:A102"/>
+    <mergeCell ref="A103:A108"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L30 G42 F43:G115 D2:D115 F2:G41 E2:E32 E34:E115">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L30 G42:G43 F44:G116 D2:D116 F2:G41 E2:E32 E34:E116">
       <formula1>"O, "</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Re-update Report 3 - Software Requirement Specification.docx (12 usecase) #LongDB
</commit_message>
<xml_diff>
--- a/wiki/report/Tasksheet.xlsx
+++ b/wiki/report/Tasksheet.xlsx
@@ -844,6 +844,17 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="9"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -874,17 +885,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="9"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1190,8 +1190,8 @@
   <dimension ref="A1:L118"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="12" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G42" sqref="G42"/>
+      <pane ySplit="12" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1248,10 +1248,10 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75" hidden="1">
-      <c r="A2" s="49">
+      <c r="A2" s="54">
         <v>1</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="54" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -1270,8 +1270,8 @@
       <c r="L2" s="30"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" hidden="1">
-      <c r="A3" s="50"/>
-      <c r="B3" s="50"/>
+      <c r="A3" s="55"/>
+      <c r="B3" s="55"/>
       <c r="C3" s="4" t="s">
         <v>45</v>
       </c>
@@ -1288,8 +1288,8 @@
       <c r="L3" s="30"/>
     </row>
     <row r="4" spans="1:12" ht="15.75" hidden="1">
-      <c r="A4" s="50"/>
-      <c r="B4" s="50"/>
+      <c r="A4" s="55"/>
+      <c r="B4" s="55"/>
       <c r="C4" s="4" t="s">
         <v>46</v>
       </c>
@@ -1306,8 +1306,8 @@
       <c r="L4" s="30"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" hidden="1">
-      <c r="A5" s="50"/>
-      <c r="B5" s="50"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="55"/>
       <c r="C5" s="4" t="s">
         <v>47</v>
       </c>
@@ -1326,8 +1326,8 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" hidden="1">
-      <c r="A6" s="50"/>
-      <c r="B6" s="50"/>
+      <c r="A6" s="55"/>
+      <c r="B6" s="55"/>
       <c r="C6" s="4" t="s">
         <v>12</v>
       </c>
@@ -1342,8 +1342,8 @@
       <c r="L6" s="30"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" hidden="1">
-      <c r="A7" s="50"/>
-      <c r="B7" s="50"/>
+      <c r="A7" s="55"/>
+      <c r="B7" s="55"/>
       <c r="C7" s="4" t="s">
         <v>13</v>
       </c>
@@ -1358,10 +1358,10 @@
       <c r="L7" s="30"/>
     </row>
     <row r="8" spans="1:12" ht="15.75" hidden="1">
-      <c r="A8" s="50">
+      <c r="A8" s="55">
         <v>2</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="55" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -1378,8 +1378,8 @@
       <c r="L8" s="30"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" hidden="1">
-      <c r="A9" s="50"/>
-      <c r="B9" s="50"/>
+      <c r="A9" s="55"/>
+      <c r="B9" s="55"/>
       <c r="C9" s="4" t="s">
         <v>10</v>
       </c>
@@ -1394,8 +1394,8 @@
       <c r="L9" s="30"/>
     </row>
     <row r="10" spans="1:12" ht="15.75" hidden="1">
-      <c r="A10" s="50"/>
-      <c r="B10" s="50"/>
+      <c r="A10" s="55"/>
+      <c r="B10" s="55"/>
       <c r="C10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1410,8 +1410,8 @@
       <c r="L10" s="30"/>
     </row>
     <row r="11" spans="1:12" ht="15.75" hidden="1">
-      <c r="A11" s="50"/>
-      <c r="B11" s="50"/>
+      <c r="A11" s="55"/>
+      <c r="B11" s="55"/>
       <c r="C11" s="4" t="s">
         <v>15</v>
       </c>
@@ -1426,8 +1426,8 @@
       <c r="L11" s="30"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" hidden="1">
-      <c r="A12" s="50"/>
-      <c r="B12" s="50"/>
+      <c r="A12" s="55"/>
+      <c r="B12" s="55"/>
       <c r="C12" s="4" t="s">
         <v>14</v>
       </c>
@@ -1442,10 +1442,10 @@
       <c r="L12" s="30"/>
     </row>
     <row r="13" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A13" s="47">
+      <c r="A13" s="52">
         <v>3</v>
       </c>
-      <c r="B13" s="51" t="s">
+      <c r="B13" s="56" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="24" t="s">
@@ -1462,8 +1462,8 @@
       <c r="L13" s="31"/>
     </row>
     <row r="14" spans="1:12" ht="15.75">
-      <c r="A14" s="48"/>
-      <c r="B14" s="52"/>
+      <c r="A14" s="53"/>
+      <c r="B14" s="57"/>
       <c r="C14" s="22" t="s">
         <v>70</v>
       </c>
@@ -1482,8 +1482,8 @@
       <c r="L14" s="31"/>
     </row>
     <row r="15" spans="1:12" ht="15.75">
-      <c r="A15" s="48"/>
-      <c r="B15" s="52"/>
+      <c r="A15" s="53"/>
+      <c r="B15" s="57"/>
       <c r="C15" s="22" t="s">
         <v>71</v>
       </c>
@@ -1502,8 +1502,8 @@
       <c r="L15" s="31"/>
     </row>
     <row r="16" spans="1:12" ht="15.75">
-      <c r="A16" s="48"/>
-      <c r="B16" s="52"/>
+      <c r="A16" s="53"/>
+      <c r="B16" s="57"/>
       <c r="C16" s="22" t="s">
         <v>72</v>
       </c>
@@ -1522,8 +1522,8 @@
       <c r="L16" s="31"/>
     </row>
     <row r="17" spans="1:12" ht="15.75">
-      <c r="A17" s="48"/>
-      <c r="B17" s="52"/>
+      <c r="A17" s="53"/>
+      <c r="B17" s="57"/>
       <c r="C17" s="23" t="s">
         <v>73</v>
       </c>
@@ -1542,8 +1542,8 @@
       <c r="L17" s="31"/>
     </row>
     <row r="18" spans="1:12" ht="15.75">
-      <c r="A18" s="48"/>
-      <c r="B18" s="52"/>
+      <c r="A18" s="53"/>
+      <c r="B18" s="57"/>
       <c r="C18" s="5" t="s">
         <v>17</v>
       </c>
@@ -1558,8 +1558,8 @@
       <c r="L18" s="31"/>
     </row>
     <row r="19" spans="1:12" ht="15.75">
-      <c r="A19" s="48"/>
-      <c r="B19" s="52"/>
+      <c r="A19" s="53"/>
+      <c r="B19" s="57"/>
       <c r="C19" s="6" t="s">
         <v>18</v>
       </c>
@@ -1576,8 +1576,8 @@
       <c r="L19" s="31"/>
     </row>
     <row r="20" spans="1:12" ht="15.75">
-      <c r="A20" s="48"/>
-      <c r="B20" s="52"/>
+      <c r="A20" s="53"/>
+      <c r="B20" s="57"/>
       <c r="C20" s="6" t="s">
         <v>74</v>
       </c>
@@ -1596,8 +1596,8 @@
       <c r="L20" s="31"/>
     </row>
     <row r="21" spans="1:12" ht="15.75">
-      <c r="A21" s="48"/>
-      <c r="B21" s="52"/>
+      <c r="A21" s="53"/>
+      <c r="B21" s="57"/>
       <c r="C21" s="7" t="s">
         <v>19</v>
       </c>
@@ -1612,8 +1612,8 @@
       <c r="L21" s="31"/>
     </row>
     <row r="22" spans="1:12" ht="15.75">
-      <c r="A22" s="48"/>
-      <c r="B22" s="52"/>
+      <c r="A22" s="53"/>
+      <c r="B22" s="57"/>
       <c r="C22" s="27" t="s">
         <v>82</v>
       </c>
@@ -1632,8 +1632,8 @@
       <c r="L22" s="31"/>
     </row>
     <row r="23" spans="1:12" ht="15.75">
-      <c r="A23" s="48"/>
-      <c r="B23" s="52"/>
+      <c r="A23" s="53"/>
+      <c r="B23" s="57"/>
       <c r="C23" s="41" t="s">
         <v>83</v>
       </c>
@@ -1652,8 +1652,8 @@
       <c r="L23" s="42"/>
     </row>
     <row r="24" spans="1:12" ht="15.75">
-      <c r="A24" s="48"/>
-      <c r="B24" s="52"/>
+      <c r="A24" s="53"/>
+      <c r="B24" s="57"/>
       <c r="C24" s="28" t="s">
         <v>84</v>
       </c>
@@ -1674,8 +1674,8 @@
       <c r="L24" s="31"/>
     </row>
     <row r="25" spans="1:12" ht="15.75">
-      <c r="A25" s="48"/>
-      <c r="B25" s="52"/>
+      <c r="A25" s="53"/>
+      <c r="B25" s="57"/>
       <c r="C25" s="28" t="s">
         <v>85</v>
       </c>
@@ -1696,8 +1696,8 @@
       <c r="L25" s="31"/>
     </row>
     <row r="26" spans="1:12" ht="15.75">
-      <c r="A26" s="48"/>
-      <c r="B26" s="52"/>
+      <c r="A26" s="53"/>
+      <c r="B26" s="57"/>
       <c r="C26" s="41" t="s">
         <v>86</v>
       </c>
@@ -1716,8 +1716,8 @@
       <c r="L26" s="42"/>
     </row>
     <row r="27" spans="1:12" ht="15.75">
-      <c r="A27" s="48"/>
-      <c r="B27" s="52"/>
+      <c r="A27" s="53"/>
+      <c r="B27" s="57"/>
       <c r="C27" s="28" t="s">
         <v>87</v>
       </c>
@@ -1738,8 +1738,8 @@
       <c r="L27" s="31"/>
     </row>
     <row r="28" spans="1:12" ht="15.75">
-      <c r="A28" s="48"/>
-      <c r="B28" s="52"/>
+      <c r="A28" s="53"/>
+      <c r="B28" s="57"/>
       <c r="C28" s="28" t="s">
         <v>88</v>
       </c>
@@ -1760,8 +1760,8 @@
       <c r="L28" s="31"/>
     </row>
     <row r="29" spans="1:12" ht="15.75">
-      <c r="A29" s="48"/>
-      <c r="B29" s="52"/>
+      <c r="A29" s="53"/>
+      <c r="B29" s="57"/>
       <c r="C29" s="28" t="s">
         <v>89</v>
       </c>
@@ -1782,8 +1782,8 @@
       <c r="L29" s="31"/>
     </row>
     <row r="30" spans="1:12" ht="15.75">
-      <c r="A30" s="48"/>
-      <c r="B30" s="52"/>
+      <c r="A30" s="53"/>
+      <c r="B30" s="57"/>
       <c r="C30" s="28" t="s">
         <v>90</v>
       </c>
@@ -1804,8 +1804,8 @@
       <c r="L30" s="31"/>
     </row>
     <row r="31" spans="1:12" ht="15.75">
-      <c r="A31" s="48"/>
-      <c r="B31" s="52"/>
+      <c r="A31" s="53"/>
+      <c r="B31" s="57"/>
       <c r="C31" s="29" t="s">
         <v>91</v>
       </c>
@@ -1826,8 +1826,8 @@
       <c r="L31" s="32"/>
     </row>
     <row r="32" spans="1:12" ht="15.75">
-      <c r="A32" s="48"/>
-      <c r="B32" s="52"/>
+      <c r="A32" s="53"/>
+      <c r="B32" s="57"/>
       <c r="C32" s="29" t="s">
         <v>92</v>
       </c>
@@ -1848,8 +1848,8 @@
       <c r="L32" s="32"/>
     </row>
     <row r="33" spans="1:12" ht="15.75">
-      <c r="A33" s="48"/>
-      <c r="B33" s="52"/>
+      <c r="A33" s="53"/>
+      <c r="B33" s="57"/>
       <c r="C33" s="29" t="s">
         <v>93</v>
       </c>
@@ -1869,8 +1869,8 @@
       <c r="L33" s="32"/>
     </row>
     <row r="34" spans="1:12" ht="15.75">
-      <c r="A34" s="48"/>
-      <c r="B34" s="52"/>
+      <c r="A34" s="53"/>
+      <c r="B34" s="57"/>
       <c r="C34" s="29" t="s">
         <v>109</v>
       </c>
@@ -1891,8 +1891,8 @@
       <c r="L34" s="32"/>
     </row>
     <row r="35" spans="1:12" ht="15.75">
-      <c r="A35" s="48"/>
-      <c r="B35" s="52"/>
+      <c r="A35" s="53"/>
+      <c r="B35" s="57"/>
       <c r="C35" s="29" t="s">
         <v>94</v>
       </c>
@@ -1913,8 +1913,8 @@
       <c r="L35" s="32"/>
     </row>
     <row r="36" spans="1:12" ht="15.75">
-      <c r="A36" s="48"/>
-      <c r="B36" s="52"/>
+      <c r="A36" s="53"/>
+      <c r="B36" s="57"/>
       <c r="C36" s="29" t="s">
         <v>95</v>
       </c>
@@ -1935,8 +1935,8 @@
       <c r="L36" s="32"/>
     </row>
     <row r="37" spans="1:12" ht="15.75">
-      <c r="A37" s="48"/>
-      <c r="B37" s="52"/>
+      <c r="A37" s="53"/>
+      <c r="B37" s="57"/>
       <c r="C37" s="41" t="s">
         <v>96</v>
       </c>
@@ -1955,8 +1955,8 @@
       <c r="L37" s="44"/>
     </row>
     <row r="38" spans="1:12" ht="15.75">
-      <c r="A38" s="48"/>
-      <c r="B38" s="52"/>
+      <c r="A38" s="53"/>
+      <c r="B38" s="57"/>
       <c r="C38" s="29" t="s">
         <v>97</v>
       </c>
@@ -1977,8 +1977,8 @@
       <c r="L38" s="32"/>
     </row>
     <row r="39" spans="1:12" ht="15.75">
-      <c r="A39" s="48"/>
-      <c r="B39" s="52"/>
+      <c r="A39" s="53"/>
+      <c r="B39" s="57"/>
       <c r="C39" s="29" t="s">
         <v>98</v>
       </c>
@@ -1999,8 +1999,8 @@
       <c r="L39" s="32"/>
     </row>
     <row r="40" spans="1:12" ht="15.75">
-      <c r="A40" s="48"/>
-      <c r="B40" s="52"/>
+      <c r="A40" s="53"/>
+      <c r="B40" s="57"/>
       <c r="C40" s="29" t="s">
         <v>99</v>
       </c>
@@ -2021,8 +2021,8 @@
       <c r="L40" s="32"/>
     </row>
     <row r="41" spans="1:12" ht="15.75">
-      <c r="A41" s="48"/>
-      <c r="B41" s="52"/>
+      <c r="A41" s="53"/>
+      <c r="B41" s="57"/>
       <c r="C41" s="29" t="s">
         <v>100</v>
       </c>
@@ -2043,29 +2043,29 @@
       <c r="L41" s="32"/>
     </row>
     <row r="42" spans="1:12" ht="15.75">
-      <c r="A42" s="48"/>
-      <c r="B42" s="52"/>
-      <c r="C42" s="57" t="s">
+      <c r="A42" s="53"/>
+      <c r="B42" s="57"/>
+      <c r="C42" s="47" t="s">
         <v>101</v>
       </c>
-      <c r="D42" s="58"/>
-      <c r="E42" s="58" t="s">
-        <v>8</v>
-      </c>
-      <c r="G42" s="58"/>
-      <c r="H42" s="59"/>
-      <c r="I42" s="60"/>
-      <c r="J42" s="61">
-        <v>41680</v>
-      </c>
-      <c r="K42" s="60" t="s">
+      <c r="D42" s="48"/>
+      <c r="E42" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="G42" s="48"/>
+      <c r="H42" s="49"/>
+      <c r="I42" s="50"/>
+      <c r="J42" s="51">
+        <v>41680</v>
+      </c>
+      <c r="K42" s="50" t="s">
         <v>125</v>
       </c>
       <c r="L42" s="32"/>
     </row>
     <row r="43" spans="1:12" ht="15.75">
-      <c r="A43" s="48"/>
-      <c r="B43" s="52"/>
+      <c r="A43" s="53"/>
+      <c r="B43" s="57"/>
       <c r="C43" s="29" t="s">
         <v>126</v>
       </c>
@@ -2077,17 +2077,17 @@
       <c r="G43" s="35"/>
       <c r="H43" s="38"/>
       <c r="I43" s="14"/>
-      <c r="J43" s="61">
-        <v>41680</v>
-      </c>
-      <c r="K43" s="60" t="s">
+      <c r="J43" s="51">
+        <v>41680</v>
+      </c>
+      <c r="K43" s="50" t="s">
         <v>125</v>
       </c>
       <c r="L43" s="32"/>
     </row>
     <row r="44" spans="1:12" ht="15.75">
-      <c r="A44" s="48"/>
-      <c r="B44" s="52"/>
+      <c r="A44" s="53"/>
+      <c r="B44" s="57"/>
       <c r="C44" s="39" t="s">
         <v>109</v>
       </c>
@@ -2108,8 +2108,8 @@
       <c r="L44" s="32"/>
     </row>
     <row r="45" spans="1:12" ht="15.75">
-      <c r="A45" s="48"/>
-      <c r="B45" s="52"/>
+      <c r="A45" s="53"/>
+      <c r="B45" s="57"/>
       <c r="C45" s="41" t="s">
         <v>102</v>
       </c>
@@ -2128,8 +2128,8 @@
       <c r="L45" s="44"/>
     </row>
     <row r="46" spans="1:12" ht="15.75">
-      <c r="A46" s="48"/>
-      <c r="B46" s="52"/>
+      <c r="A46" s="53"/>
+      <c r="B46" s="57"/>
       <c r="C46" s="29" t="s">
         <v>103</v>
       </c>
@@ -2150,8 +2150,8 @@
       <c r="L46" s="32"/>
     </row>
     <row r="47" spans="1:12" ht="15.75">
-      <c r="A47" s="48"/>
-      <c r="B47" s="52"/>
+      <c r="A47" s="53"/>
+      <c r="B47" s="57"/>
       <c r="C47" s="29" t="s">
         <v>104</v>
       </c>
@@ -2172,8 +2172,8 @@
       <c r="L47" s="32"/>
     </row>
     <row r="48" spans="1:12" ht="15.75">
-      <c r="A48" s="48"/>
-      <c r="B48" s="52"/>
+      <c r="A48" s="53"/>
+      <c r="B48" s="57"/>
       <c r="C48" s="29" t="s">
         <v>105</v>
       </c>
@@ -2194,8 +2194,8 @@
       <c r="L48" s="32"/>
     </row>
     <row r="49" spans="1:12" ht="15.75">
-      <c r="A49" s="48"/>
-      <c r="B49" s="52"/>
+      <c r="A49" s="53"/>
+      <c r="B49" s="57"/>
       <c r="C49" s="29" t="s">
         <v>106</v>
       </c>
@@ -2216,8 +2216,8 @@
       <c r="L49" s="32"/>
     </row>
     <row r="50" spans="1:12" ht="15.75">
-      <c r="A50" s="48"/>
-      <c r="B50" s="52"/>
+      <c r="A50" s="53"/>
+      <c r="B50" s="57"/>
       <c r="C50" s="29" t="s">
         <v>107</v>
       </c>
@@ -2238,8 +2238,8 @@
       <c r="L50" s="32"/>
     </row>
     <row r="51" spans="1:12" ht="15.75">
-      <c r="A51" s="48"/>
-      <c r="B51" s="52"/>
+      <c r="A51" s="53"/>
+      <c r="B51" s="57"/>
       <c r="C51" s="29" t="s">
         <v>108</v>
       </c>
@@ -2260,8 +2260,8 @@
       <c r="L51" s="32"/>
     </row>
     <row r="52" spans="1:12" ht="15.75">
-      <c r="A52" s="48"/>
-      <c r="B52" s="52"/>
+      <c r="A52" s="53"/>
+      <c r="B52" s="57"/>
       <c r="C52" s="29" t="s">
         <v>109</v>
       </c>
@@ -2282,8 +2282,8 @@
       <c r="L52" s="32"/>
     </row>
     <row r="53" spans="1:12" ht="15.75">
-      <c r="A53" s="48"/>
-      <c r="B53" s="52"/>
+      <c r="A53" s="53"/>
+      <c r="B53" s="57"/>
       <c r="C53" s="29" t="s">
         <v>110</v>
       </c>
@@ -2304,8 +2304,8 @@
       <c r="L53" s="32"/>
     </row>
     <row r="54" spans="1:12" ht="15.75">
-      <c r="A54" s="48"/>
-      <c r="B54" s="52"/>
+      <c r="A54" s="53"/>
+      <c r="B54" s="57"/>
       <c r="C54" s="29" t="s">
         <v>111</v>
       </c>
@@ -2326,8 +2326,8 @@
       <c r="L54" s="32"/>
     </row>
     <row r="55" spans="1:12" ht="15.75">
-      <c r="A55" s="48"/>
-      <c r="B55" s="52"/>
+      <c r="A55" s="53"/>
+      <c r="B55" s="57"/>
       <c r="C55" s="29" t="s">
         <v>112</v>
       </c>
@@ -2348,8 +2348,8 @@
       <c r="L55" s="32"/>
     </row>
     <row r="56" spans="1:12" ht="15.75">
-      <c r="A56" s="48"/>
-      <c r="B56" s="52"/>
+      <c r="A56" s="53"/>
+      <c r="B56" s="57"/>
       <c r="C56" s="29" t="s">
         <v>113</v>
       </c>
@@ -2370,8 +2370,8 @@
       <c r="L56" s="32"/>
     </row>
     <row r="57" spans="1:12" ht="15.75">
-      <c r="A57" s="48"/>
-      <c r="B57" s="52"/>
+      <c r="A57" s="53"/>
+      <c r="B57" s="57"/>
       <c r="C57" s="29" t="s">
         <v>114</v>
       </c>
@@ -2392,8 +2392,8 @@
       <c r="L57" s="32"/>
     </row>
     <row r="58" spans="1:12" ht="15.75">
-      <c r="A58" s="48"/>
-      <c r="B58" s="52"/>
+      <c r="A58" s="53"/>
+      <c r="B58" s="57"/>
       <c r="C58" s="29" t="s">
         <v>115</v>
       </c>
@@ -2414,8 +2414,8 @@
       <c r="L58" s="32"/>
     </row>
     <row r="59" spans="1:12" ht="15.75">
-      <c r="A59" s="48"/>
-      <c r="B59" s="52"/>
+      <c r="A59" s="53"/>
+      <c r="B59" s="57"/>
       <c r="C59" s="29" t="s">
         <v>116</v>
       </c>
@@ -2436,8 +2436,8 @@
       <c r="L59" s="32"/>
     </row>
     <row r="60" spans="1:12" ht="15.75">
-      <c r="A60" s="48"/>
-      <c r="B60" s="52"/>
+      <c r="A60" s="53"/>
+      <c r="B60" s="57"/>
       <c r="C60" s="29" t="s">
         <v>117</v>
       </c>
@@ -2458,8 +2458,8 @@
       <c r="L60" s="32"/>
     </row>
     <row r="61" spans="1:12" ht="15.75">
-      <c r="A61" s="48"/>
-      <c r="B61" s="52"/>
+      <c r="A61" s="53"/>
+      <c r="B61" s="57"/>
       <c r="C61" s="29" t="s">
         <v>118</v>
       </c>
@@ -2480,8 +2480,8 @@
       <c r="L61" s="32"/>
     </row>
     <row r="62" spans="1:12" ht="15.75">
-      <c r="A62" s="48"/>
-      <c r="B62" s="52"/>
+      <c r="A62" s="53"/>
+      <c r="B62" s="57"/>
       <c r="C62" s="29" t="s">
         <v>119</v>
       </c>
@@ -2502,8 +2502,8 @@
       <c r="L62" s="32"/>
     </row>
     <row r="63" spans="1:12" ht="15.75">
-      <c r="A63" s="48"/>
-      <c r="B63" s="52"/>
+      <c r="A63" s="53"/>
+      <c r="B63" s="57"/>
       <c r="C63" s="29" t="s">
         <v>120</v>
       </c>
@@ -2524,8 +2524,8 @@
       <c r="L63" s="32"/>
     </row>
     <row r="64" spans="1:12" ht="15.75">
-      <c r="A64" s="48"/>
-      <c r="B64" s="52"/>
+      <c r="A64" s="53"/>
+      <c r="B64" s="57"/>
       <c r="C64" s="29" t="s">
         <v>121</v>
       </c>
@@ -2546,8 +2546,8 @@
       <c r="L64" s="32"/>
     </row>
     <row r="65" spans="1:12" ht="15.75">
-      <c r="A65" s="48"/>
-      <c r="B65" s="52"/>
+      <c r="A65" s="53"/>
+      <c r="B65" s="57"/>
       <c r="C65" s="29" t="s">
         <v>122</v>
       </c>
@@ -2568,8 +2568,8 @@
       <c r="L65" s="32"/>
     </row>
     <row r="66" spans="1:12" ht="15.75">
-      <c r="A66" s="48"/>
-      <c r="B66" s="52"/>
+      <c r="A66" s="53"/>
+      <c r="B66" s="57"/>
       <c r="C66" s="29" t="s">
         <v>123</v>
       </c>
@@ -2590,8 +2590,8 @@
       <c r="L66" s="32"/>
     </row>
     <row r="67" spans="1:12" ht="15.75">
-      <c r="A67" s="48"/>
-      <c r="B67" s="52"/>
+      <c r="A67" s="53"/>
+      <c r="B67" s="57"/>
       <c r="C67" s="7" t="s">
         <v>21</v>
       </c>
@@ -2606,8 +2606,8 @@
       <c r="L67" s="32"/>
     </row>
     <row r="68" spans="1:12" ht="15.75">
-      <c r="A68" s="48"/>
-      <c r="B68" s="52"/>
+      <c r="A68" s="53"/>
+      <c r="B68" s="57"/>
       <c r="C68" s="8" t="s">
         <v>22</v>
       </c>
@@ -2622,8 +2622,8 @@
       <c r="L68" s="32"/>
     </row>
     <row r="69" spans="1:12" ht="15.75">
-      <c r="A69" s="49"/>
-      <c r="B69" s="53"/>
+      <c r="A69" s="54"/>
+      <c r="B69" s="58"/>
       <c r="C69" s="8" t="s">
         <v>23</v>
       </c>
@@ -2638,10 +2638,10 @@
       <c r="L69" s="32"/>
     </row>
     <row r="70" spans="1:12" ht="15.75">
-      <c r="A70" s="47">
+      <c r="A70" s="52">
         <v>4</v>
       </c>
-      <c r="B70" s="47" t="s">
+      <c r="B70" s="52" t="s">
         <v>6</v>
       </c>
       <c r="C70" s="8" t="s">
@@ -2658,8 +2658,8 @@
       <c r="L70" s="32"/>
     </row>
     <row r="71" spans="1:12" ht="15.75">
-      <c r="A71" s="48"/>
-      <c r="B71" s="48"/>
+      <c r="A71" s="53"/>
+      <c r="B71" s="53"/>
       <c r="C71" s="9" t="s">
         <v>25</v>
       </c>
@@ -2674,8 +2674,8 @@
       <c r="L71" s="32"/>
     </row>
     <row r="72" spans="1:12" ht="15.75">
-      <c r="A72" s="48"/>
-      <c r="B72" s="48"/>
+      <c r="A72" s="53"/>
+      <c r="B72" s="53"/>
       <c r="C72" s="4" t="s">
         <v>26</v>
       </c>
@@ -2690,8 +2690,8 @@
       <c r="L72" s="32"/>
     </row>
     <row r="73" spans="1:12" ht="15.75">
-      <c r="A73" s="48"/>
-      <c r="B73" s="48"/>
+      <c r="A73" s="53"/>
+      <c r="B73" s="53"/>
       <c r="C73" s="4" t="s">
         <v>53</v>
       </c>
@@ -2706,8 +2706,8 @@
       <c r="L73" s="32"/>
     </row>
     <row r="74" spans="1:12" ht="15.75">
-      <c r="A74" s="48"/>
-      <c r="B74" s="48"/>
+      <c r="A74" s="53"/>
+      <c r="B74" s="53"/>
       <c r="C74" s="10" t="s">
         <v>54</v>
       </c>
@@ -2722,8 +2722,8 @@
       <c r="L74" s="32"/>
     </row>
     <row r="75" spans="1:12" ht="15.75">
-      <c r="A75" s="48"/>
-      <c r="B75" s="48"/>
+      <c r="A75" s="53"/>
+      <c r="B75" s="53"/>
       <c r="C75" s="11" t="s">
         <v>55</v>
       </c>
@@ -2738,8 +2738,8 @@
       <c r="L75" s="32"/>
     </row>
     <row r="76" spans="1:12" ht="15.75">
-      <c r="A76" s="48"/>
-      <c r="B76" s="48"/>
+      <c r="A76" s="53"/>
+      <c r="B76" s="53"/>
       <c r="C76" s="11" t="s">
         <v>56</v>
       </c>
@@ -2754,8 +2754,8 @@
       <c r="L76" s="32"/>
     </row>
     <row r="77" spans="1:12" ht="15.75">
-      <c r="A77" s="48"/>
-      <c r="B77" s="48"/>
+      <c r="A77" s="53"/>
+      <c r="B77" s="53"/>
       <c r="C77" s="12" t="s">
         <v>27</v>
       </c>
@@ -2770,8 +2770,8 @@
       <c r="L77" s="32"/>
     </row>
     <row r="78" spans="1:12" ht="15.75">
-      <c r="A78" s="48"/>
-      <c r="B78" s="48"/>
+      <c r="A78" s="53"/>
+      <c r="B78" s="53"/>
       <c r="C78" s="10" t="s">
         <v>28</v>
       </c>
@@ -2786,8 +2786,8 @@
       <c r="L78" s="32"/>
     </row>
     <row r="79" spans="1:12" ht="15.75">
-      <c r="A79" s="48"/>
-      <c r="B79" s="48"/>
+      <c r="A79" s="53"/>
+      <c r="B79" s="53"/>
       <c r="C79" s="11" t="s">
         <v>29</v>
       </c>
@@ -2802,8 +2802,8 @@
       <c r="L79" s="32"/>
     </row>
     <row r="80" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A80" s="48"/>
-      <c r="B80" s="48"/>
+      <c r="A80" s="53"/>
+      <c r="B80" s="53"/>
       <c r="C80" s="11" t="s">
         <v>30</v>
       </c>
@@ -2818,8 +2818,8 @@
       <c r="L80" s="32"/>
     </row>
     <row r="81" spans="1:12" ht="15.75">
-      <c r="A81" s="48"/>
-      <c r="B81" s="48"/>
+      <c r="A81" s="53"/>
+      <c r="B81" s="53"/>
       <c r="C81" s="13" t="s">
         <v>31</v>
       </c>
@@ -2834,8 +2834,8 @@
       <c r="L81" s="32"/>
     </row>
     <row r="82" spans="1:12" ht="15.75">
-      <c r="A82" s="48"/>
-      <c r="B82" s="48"/>
+      <c r="A82" s="53"/>
+      <c r="B82" s="53"/>
       <c r="C82" s="8" t="s">
         <v>50</v>
       </c>
@@ -2850,8 +2850,8 @@
       <c r="L82" s="32"/>
     </row>
     <row r="83" spans="1:12" ht="15.75">
-      <c r="A83" s="48"/>
-      <c r="B83" s="48"/>
+      <c r="A83" s="53"/>
+      <c r="B83" s="53"/>
       <c r="C83" s="8" t="s">
         <v>51</v>
       </c>
@@ -2866,8 +2866,8 @@
       <c r="L83" s="32"/>
     </row>
     <row r="84" spans="1:12" ht="15.75">
-      <c r="A84" s="49"/>
-      <c r="B84" s="49"/>
+      <c r="A84" s="54"/>
+      <c r="B84" s="54"/>
       <c r="C84" s="8" t="s">
         <v>52</v>
       </c>
@@ -2882,10 +2882,10 @@
       <c r="L84" s="32"/>
     </row>
     <row r="85" spans="1:12" ht="15.75">
-      <c r="A85" s="54">
+      <c r="A85" s="59">
         <v>5</v>
       </c>
-      <c r="B85" s="47" t="s">
+      <c r="B85" s="52" t="s">
         <v>58</v>
       </c>
       <c r="C85" s="13" t="s">
@@ -2902,8 +2902,8 @@
       <c r="L85" s="32"/>
     </row>
     <row r="86" spans="1:12" ht="15.75">
-      <c r="A86" s="55"/>
-      <c r="B86" s="48"/>
+      <c r="A86" s="60"/>
+      <c r="B86" s="53"/>
       <c r="C86" s="13" t="s">
         <v>49</v>
       </c>
@@ -2918,8 +2918,8 @@
       <c r="L86" s="32"/>
     </row>
     <row r="87" spans="1:12" ht="15.75">
-      <c r="A87" s="55"/>
-      <c r="B87" s="48"/>
+      <c r="A87" s="60"/>
+      <c r="B87" s="53"/>
       <c r="C87" s="5" t="s">
         <v>40</v>
       </c>
@@ -2934,8 +2934,8 @@
       <c r="L87" s="32"/>
     </row>
     <row r="88" spans="1:12" ht="15.75">
-      <c r="A88" s="55"/>
-      <c r="B88" s="48"/>
+      <c r="A88" s="60"/>
+      <c r="B88" s="53"/>
       <c r="C88" s="5" t="s">
         <v>32</v>
       </c>
@@ -2950,8 +2950,8 @@
       <c r="L88" s="32"/>
     </row>
     <row r="89" spans="1:12" ht="15.75">
-      <c r="A89" s="55"/>
-      <c r="B89" s="48"/>
+      <c r="A89" s="60"/>
+      <c r="B89" s="53"/>
       <c r="C89" s="11" t="s">
         <v>34</v>
       </c>
@@ -2966,8 +2966,8 @@
       <c r="L89" s="32"/>
     </row>
     <row r="90" spans="1:12" ht="15.75">
-      <c r="A90" s="55"/>
-      <c r="B90" s="48"/>
+      <c r="A90" s="60"/>
+      <c r="B90" s="53"/>
       <c r="C90" s="11" t="s">
         <v>35</v>
       </c>
@@ -2982,8 +2982,8 @@
       <c r="L90" s="32"/>
     </row>
     <row r="91" spans="1:12" ht="15.75">
-      <c r="A91" s="55"/>
-      <c r="B91" s="48"/>
+      <c r="A91" s="60"/>
+      <c r="B91" s="53"/>
       <c r="C91" s="5" t="s">
         <v>33</v>
       </c>
@@ -2998,8 +2998,8 @@
       <c r="L91" s="32"/>
     </row>
     <row r="92" spans="1:12" ht="15.75">
-      <c r="A92" s="55"/>
-      <c r="B92" s="48"/>
+      <c r="A92" s="60"/>
+      <c r="B92" s="53"/>
       <c r="C92" s="11" t="s">
         <v>34</v>
       </c>
@@ -3014,8 +3014,8 @@
       <c r="L92" s="32"/>
     </row>
     <row r="93" spans="1:12" ht="15.75">
-      <c r="A93" s="55"/>
-      <c r="B93" s="48"/>
+      <c r="A93" s="60"/>
+      <c r="B93" s="53"/>
       <c r="C93" s="11" t="s">
         <v>35</v>
       </c>
@@ -3030,8 +3030,8 @@
       <c r="L93" s="32"/>
     </row>
     <row r="94" spans="1:12" ht="15.75">
-      <c r="A94" s="55"/>
-      <c r="B94" s="48"/>
+      <c r="A94" s="60"/>
+      <c r="B94" s="53"/>
       <c r="C94" s="4" t="s">
         <v>59</v>
       </c>
@@ -3046,8 +3046,8 @@
       <c r="L94" s="32"/>
     </row>
     <row r="95" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A95" s="55"/>
-      <c r="B95" s="48"/>
+      <c r="A95" s="60"/>
+      <c r="B95" s="53"/>
       <c r="C95" s="13" t="s">
         <v>36</v>
       </c>
@@ -3062,8 +3062,8 @@
       <c r="L95" s="32"/>
     </row>
     <row r="96" spans="1:12" ht="15.75">
-      <c r="A96" s="55"/>
-      <c r="B96" s="48"/>
+      <c r="A96" s="60"/>
+      <c r="B96" s="53"/>
       <c r="C96" s="11" t="s">
         <v>20</v>
       </c>
@@ -3078,8 +3078,8 @@
       <c r="L96" s="32"/>
     </row>
     <row r="97" spans="1:12" ht="15.75">
-      <c r="A97" s="55"/>
-      <c r="B97" s="48"/>
+      <c r="A97" s="60"/>
+      <c r="B97" s="53"/>
       <c r="C97" s="11" t="s">
         <v>38</v>
       </c>
@@ -3094,8 +3094,8 @@
       <c r="L97" s="32"/>
     </row>
     <row r="98" spans="1:12" ht="15.75">
-      <c r="A98" s="55"/>
-      <c r="B98" s="48"/>
+      <c r="A98" s="60"/>
+      <c r="B98" s="53"/>
       <c r="C98" s="11" t="s">
         <v>39</v>
       </c>
@@ -3110,8 +3110,8 @@
       <c r="L98" s="32"/>
     </row>
     <row r="99" spans="1:12" ht="15.75">
-      <c r="A99" s="55"/>
-      <c r="B99" s="48"/>
+      <c r="A99" s="60"/>
+      <c r="B99" s="53"/>
       <c r="C99" s="13" t="s">
         <v>37</v>
       </c>
@@ -3126,8 +3126,8 @@
       <c r="L99" s="32"/>
     </row>
     <row r="100" spans="1:12" ht="15.75">
-      <c r="A100" s="55"/>
-      <c r="B100" s="48"/>
+      <c r="A100" s="60"/>
+      <c r="B100" s="53"/>
       <c r="C100" s="11" t="s">
         <v>20</v>
       </c>
@@ -3142,8 +3142,8 @@
       <c r="L100" s="32"/>
     </row>
     <row r="101" spans="1:12" ht="15.75">
-      <c r="A101" s="55"/>
-      <c r="B101" s="48"/>
+      <c r="A101" s="60"/>
+      <c r="B101" s="53"/>
       <c r="C101" s="11" t="s">
         <v>38</v>
       </c>
@@ -3158,8 +3158,8 @@
       <c r="L101" s="32"/>
     </row>
     <row r="102" spans="1:12" ht="15.75">
-      <c r="A102" s="56"/>
-      <c r="B102" s="49"/>
+      <c r="A102" s="61"/>
+      <c r="B102" s="54"/>
       <c r="C102" s="13" t="s">
         <v>57</v>
       </c>
@@ -3174,10 +3174,10 @@
       <c r="L102" s="32"/>
     </row>
     <row r="103" spans="1:12" ht="15.75">
-      <c r="A103" s="54">
+      <c r="A103" s="59">
         <v>6</v>
       </c>
-      <c r="B103" s="47" t="s">
+      <c r="B103" s="52" t="s">
         <v>7</v>
       </c>
       <c r="C103" s="11" t="s">
@@ -3194,8 +3194,8 @@
       <c r="L103" s="32"/>
     </row>
     <row r="104" spans="1:12" ht="15.75">
-      <c r="A104" s="55"/>
-      <c r="B104" s="48"/>
+      <c r="A104" s="60"/>
+      <c r="B104" s="53"/>
       <c r="C104" s="11" t="s">
         <v>38</v>
       </c>
@@ -3210,8 +3210,8 @@
       <c r="L104" s="32"/>
     </row>
     <row r="105" spans="1:12" ht="15.75">
-      <c r="A105" s="55"/>
-      <c r="B105" s="48"/>
+      <c r="A105" s="60"/>
+      <c r="B105" s="53"/>
       <c r="C105" s="13" t="s">
         <v>41</v>
       </c>
@@ -3226,8 +3226,8 @@
       <c r="L105" s="32"/>
     </row>
     <row r="106" spans="1:12" ht="15.75">
-      <c r="A106" s="55"/>
-      <c r="B106" s="48"/>
+      <c r="A106" s="60"/>
+      <c r="B106" s="53"/>
       <c r="C106" s="13" t="s">
         <v>42</v>
       </c>
@@ -3242,8 +3242,8 @@
       <c r="L106" s="32"/>
     </row>
     <row r="107" spans="1:12" ht="15.75">
-      <c r="A107" s="55"/>
-      <c r="B107" s="48"/>
+      <c r="A107" s="60"/>
+      <c r="B107" s="53"/>
       <c r="C107" s="11" t="s">
         <v>20</v>
       </c>
@@ -3258,8 +3258,8 @@
       <c r="L107" s="32"/>
     </row>
     <row r="108" spans="1:12" ht="15.75">
-      <c r="A108" s="56"/>
-      <c r="B108" s="49"/>
+      <c r="A108" s="61"/>
+      <c r="B108" s="54"/>
       <c r="C108" s="11" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
Update Tasksheet.xlsx: sequence diagram task #LongDB
</commit_message>
<xml_diff>
--- a/wiki/report/Tasksheet.xlsx
+++ b/wiki/report/Tasksheet.xlsx
@@ -764,7 +764,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -922,6 +922,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1228,8 +1231,8 @@
   <dimension ref="A1:L125"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="12" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L74" sqref="L74"/>
+      <pane ySplit="12" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G89" sqref="G89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2998,11 +3001,11 @@
         <v>132</v>
       </c>
       <c r="D86" s="26"/>
-      <c r="E86" s="26" t="s">
-        <v>8</v>
-      </c>
+      <c r="E86" s="7"/>
       <c r="F86" s="26"/>
-      <c r="G86" s="26"/>
+      <c r="G86" s="26" t="s">
+        <v>8</v>
+      </c>
       <c r="H86" s="31"/>
       <c r="I86" s="32"/>
       <c r="J86" s="38">
@@ -3018,11 +3021,11 @@
         <v>133</v>
       </c>
       <c r="D87" s="26"/>
-      <c r="E87" s="26" t="s">
-        <v>8</v>
-      </c>
+      <c r="E87" s="7"/>
       <c r="F87" s="26"/>
-      <c r="G87" s="26"/>
+      <c r="G87" s="26" t="s">
+        <v>8</v>
+      </c>
       <c r="H87" s="31"/>
       <c r="I87" s="32"/>
       <c r="J87" s="38">
@@ -3038,7 +3041,7 @@
         <v>116</v>
       </c>
       <c r="D88" s="26"/>
-      <c r="E88" s="26"/>
+      <c r="E88" s="64"/>
       <c r="F88" s="26"/>
       <c r="G88" s="26"/>
       <c r="H88" s="31"/>
@@ -3689,7 +3692,7 @@
     <mergeCell ref="A112:A117"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G42:G43 F2:G41 E2:E32 L2:L117 D2:D125 F44:G125 E34:E125">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G42:G43 F2:G41 E2:E32 L2:L117 D2:D125 F44:G125 E34:E85 E88:E125">
       <formula1>"O, "</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>